<commit_message>
added unit mix calculation
</commit_message>
<xml_diff>
--- a/sandbox/Yield Matrix - Copy.xlsx
+++ b/sandbox/Yield Matrix - Copy.xlsx
@@ -14,17 +14,17 @@
   <sheets>
     <sheet name="Scheme Summary" sheetId="1" r:id="rId1"/>
     <sheet name="UnitSummary" sheetId="31" r:id="rId2"/>
-    <sheet name="UnitMix" sheetId="27" r:id="rId3"/>
+    <sheet name="UnitMix" sheetId="32" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Scheme Summary'!$A$1:$V$32</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Scheme Summary'!$A$1:$V$33</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>TOTAL</t>
   </si>
@@ -38,31 +38,13 @@
     <t>Unit Area (+/-)</t>
   </si>
   <si>
-    <t>TOTAL RENTABLE</t>
-  </si>
-  <si>
     <t xml:space="preserve">Individual Unit Mix  </t>
   </si>
   <si>
     <t xml:space="preserve">UNIT MIX </t>
   </si>
   <si>
-    <t>1 BEDROOM</t>
-  </si>
-  <si>
-    <t>3 BEDROOM</t>
-  </si>
-  <si>
-    <t>OPEN 1 BEDROOM</t>
-  </si>
-  <si>
     <t>Average Unit Area</t>
-  </si>
-  <si>
-    <t>2 BEDROOM + 1 BATH</t>
-  </si>
-  <si>
-    <t>2 BEDROOM + 2 BATH</t>
   </si>
   <si>
     <t>Open 1 Bedroom</t>
@@ -94,6 +76,12 @@
   <si>
     <t>Den</t>
   </si>
+  <si>
+    <t>Total Rentable Area</t>
+  </si>
+  <si>
+    <t>Rentable Per Type</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +90,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +153,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -187,25 +191,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.79998168889431442"/>
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF99"/>
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC66"/>
+        <fgColor theme="6" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -231,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -288,55 +292,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -349,6 +314,75 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -667,195 +701,195 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:V32"/>
+  <dimension ref="A1:CD35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="K31" sqref="J31:K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.140625" customWidth="1"/>
-    <col min="2" max="8" width="15.7109375" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" style="1" customWidth="1"/>
-    <col min="10" max="20" width="15.7109375" customWidth="1"/>
+    <col min="2" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.7109375" style="1" customWidth="1"/>
+    <col min="10" max="20" width="12.7109375" customWidth="1"/>
     <col min="21" max="21" width="4.28515625" customWidth="1"/>
     <col min="22" max="22" width="10.42578125" customWidth="1"/>
     <col min="23" max="24" width="10.7109375" customWidth="1"/>
     <col min="25" max="31" width="9.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="U1" s="10"/>
     </row>
-    <row r="2" spans="1:21" s="43" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="42" t="str">
+    <row r="2" spans="1:82" s="28" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="str">
         <f>IF(UnitSummary!A1&lt;&gt;"",UnitSummary!A1,"")</f>
         <v/>
       </c>
-      <c r="B2" s="42" t="str">
+      <c r="B2" s="27" t="str">
         <f>IF(UnitSummary!B1&lt;&gt;"",UnitSummary!B1,"")</f>
         <v>Open 1 Bedroom</v>
       </c>
-      <c r="C2" s="42" t="str">
+      <c r="C2" s="27" t="str">
         <f>IF(UnitSummary!C1&lt;&gt;"",UnitSummary!C1,"")</f>
         <v>1 Bedroom + Den</v>
       </c>
-      <c r="D2" s="42" t="str">
+      <c r="D2" s="27" t="str">
         <f>IF(UnitSummary!D1&lt;&gt;"",UnitSummary!D1,"")</f>
         <v>2 Bedroom</v>
       </c>
-      <c r="E2" s="42" t="str">
+      <c r="E2" s="27" t="str">
         <f>IF(UnitSummary!E1&lt;&gt;"",UnitSummary!E1,"")</f>
         <v/>
       </c>
-      <c r="F2" s="42" t="str">
+      <c r="F2" s="27" t="str">
         <f>IF(UnitSummary!F1&lt;&gt;"",UnitSummary!F1,"")</f>
         <v/>
       </c>
-      <c r="G2" s="42" t="str">
+      <c r="G2" s="27" t="str">
         <f>IF(UnitSummary!G1&lt;&gt;"",UnitSummary!G1,"")</f>
         <v/>
       </c>
-      <c r="H2" s="42" t="str">
+      <c r="H2" s="27" t="str">
         <f>IF(UnitSummary!H1&lt;&gt;"",UnitSummary!H1,"")</f>
         <v/>
       </c>
-      <c r="I2" s="42" t="str">
+      <c r="I2" s="27" t="str">
         <f>IF(UnitSummary!I1&lt;&gt;"",UnitSummary!I1,"")</f>
         <v/>
       </c>
-      <c r="J2" s="42" t="str">
+      <c r="J2" s="27" t="str">
         <f>IF(UnitSummary!J1&lt;&gt;"",UnitSummary!J1,"")</f>
         <v/>
       </c>
-      <c r="K2" s="42" t="str">
+      <c r="K2" s="27" t="str">
         <f>IF(UnitSummary!K1&lt;&gt;"",UnitSummary!K1,"")</f>
         <v/>
       </c>
-      <c r="L2" s="42" t="str">
+      <c r="L2" s="27" t="str">
         <f>IF(UnitSummary!L1&lt;&gt;"",UnitSummary!L1,"")</f>
         <v/>
       </c>
-      <c r="M2" s="42" t="str">
+      <c r="M2" s="27" t="str">
         <f>IF(UnitSummary!M1&lt;&gt;"",UnitSummary!M1,"")</f>
         <v/>
       </c>
-      <c r="N2" s="42" t="str">
+      <c r="N2" s="27" t="str">
         <f>IF(UnitSummary!N1&lt;&gt;"",UnitSummary!N1,"")</f>
         <v/>
       </c>
-      <c r="O2" s="42" t="str">
+      <c r="O2" s="27" t="str">
         <f>IF(UnitSummary!O1&lt;&gt;"",UnitSummary!O1,"")</f>
         <v/>
       </c>
-      <c r="P2" s="42" t="str">
+      <c r="P2" s="27" t="str">
         <f>IF(UnitSummary!P1&lt;&gt;"",UnitSummary!P1,"")</f>
         <v/>
       </c>
-      <c r="Q2" s="42" t="str">
+      <c r="Q2" s="27" t="str">
         <f>IF(UnitSummary!Q1&lt;&gt;"",UnitSummary!Q1,"")</f>
         <v/>
       </c>
-      <c r="R2" s="42" t="str">
+      <c r="R2" s="27" t="str">
         <f>IF(UnitSummary!R1&lt;&gt;"",UnitSummary!R1,"")</f>
         <v/>
       </c>
-      <c r="S2" s="42" t="str">
+      <c r="S2" s="27" t="str">
         <f>IF(UnitSummary!S1&lt;&gt;"",UnitSummary!S1,"")</f>
         <v/>
       </c>
-      <c r="T2" s="42" t="str">
+      <c r="T2" s="27" t="str">
         <f>IF(UnitSummary!T1&lt;&gt;"",UnitSummary!T1,"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="36" t="str">
+    <row r="3" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="22" t="str">
         <f>IF(UnitSummary!A6&lt;&gt;"",UnitSummary!A6,"")</f>
         <v>FLOOR</v>
       </c>
-      <c r="B3" s="36">
+      <c r="B3" s="22">
         <f>IF(UnitSummary!B6&lt;&gt;"",UnitSummary!B6,"")</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="C3" s="36">
+      <c r="C3" s="22">
         <f>IF(UnitSummary!C6&lt;&gt;"",UnitSummary!C6,"")</f>
         <v>1.2</v>
       </c>
-      <c r="D3" s="36">
+      <c r="D3" s="22">
         <f>IF(UnitSummary!D6&lt;&gt;"",UnitSummary!D6,"")</f>
         <v>2.1</v>
       </c>
-      <c r="E3" s="36" t="str">
+      <c r="E3" s="22" t="str">
         <f>IF(UnitSummary!E6&lt;&gt;"",UnitSummary!E6,"")</f>
         <v>TOTAL</v>
       </c>
-      <c r="F3" s="36" t="str">
+      <c r="F3" s="22" t="str">
         <f>IF(UnitSummary!F6&lt;&gt;"",UnitSummary!F6,"")</f>
         <v/>
       </c>
-      <c r="G3" s="36" t="str">
+      <c r="G3" s="22" t="str">
         <f>IF(UnitSummary!G6&lt;&gt;"",UnitSummary!G6,"")</f>
         <v/>
       </c>
-      <c r="H3" s="36" t="str">
+      <c r="H3" s="22" t="str">
         <f>IF(UnitSummary!H6&lt;&gt;"",UnitSummary!H6,"")</f>
         <v/>
       </c>
-      <c r="I3" s="36" t="str">
+      <c r="I3" s="22" t="str">
         <f>IF(UnitSummary!I6&lt;&gt;"",UnitSummary!I6,"")</f>
         <v/>
       </c>
-      <c r="J3" s="36" t="str">
+      <c r="J3" s="22" t="str">
         <f>IF(UnitSummary!J6&lt;&gt;"",UnitSummary!J6,"")</f>
         <v/>
       </c>
-      <c r="K3" s="36" t="str">
+      <c r="K3" s="22" t="str">
         <f>IF(UnitSummary!K6&lt;&gt;"",UnitSummary!K6,"")</f>
         <v/>
       </c>
-      <c r="L3" s="36" t="str">
+      <c r="L3" s="22" t="str">
         <f>IF(UnitSummary!L6&lt;&gt;"",UnitSummary!L6,"")</f>
         <v/>
       </c>
-      <c r="M3" s="36" t="str">
+      <c r="M3" s="22" t="str">
         <f>IF(UnitSummary!M6&lt;&gt;"",UnitSummary!M6,"")</f>
         <v/>
       </c>
-      <c r="N3" s="36" t="str">
+      <c r="N3" s="22" t="str">
         <f>IF(UnitSummary!N6&lt;&gt;"",UnitSummary!N6,"")</f>
         <v/>
       </c>
-      <c r="O3" s="36" t="str">
+      <c r="O3" s="22" t="str">
         <f>IF(UnitSummary!O6&lt;&gt;"",UnitSummary!O6,"")</f>
         <v/>
       </c>
-      <c r="P3" s="36" t="str">
+      <c r="P3" s="22" t="str">
         <f>IF(UnitSummary!P6&lt;&gt;"",UnitSummary!P6,"")</f>
         <v/>
       </c>
-      <c r="Q3" s="36" t="str">
+      <c r="Q3" s="22" t="str">
         <f>IF(UnitSummary!Q6&lt;&gt;"",UnitSummary!Q6,"")</f>
         <v/>
       </c>
-      <c r="R3" s="36" t="str">
+      <c r="R3" s="22" t="str">
         <f>IF(UnitSummary!R6&lt;&gt;"",UnitSummary!R6,"")</f>
         <v/>
       </c>
-      <c r="S3" s="36" t="str">
+      <c r="S3" s="22" t="str">
         <f>IF(UnitSummary!S6&lt;&gt;"",UnitSummary!S6,"")</f>
         <v/>
       </c>
-      <c r="T3" s="36" t="str">
+      <c r="T3" s="22" t="str">
         <f>IF(UnitSummary!T6&lt;&gt;"",UnitSummary!T6,"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>IF(UnitSummary!A7&lt;&gt;"",UnitSummary!A7,"")</f>
         <v>Level 1</v>
@@ -937,89 +971,151 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="str">
+    <row r="5" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="39" t="str">
         <f>IF(UnitSummary!A8&lt;&gt;"",UnitSummary!A8,"")</f>
         <v>Level 2</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5" s="39">
         <f>IF(UnitSummary!B8&lt;&gt;"",UnitSummary!B8,"")</f>
         <v>5</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="39">
         <f>IF(UnitSummary!C8&lt;&gt;"",UnitSummary!C8,"")</f>
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="39">
         <f>IF(UnitSummary!D8&lt;&gt;"",UnitSummary!D8,"")</f>
         <v>2</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5" s="39">
         <f>IF(UnitSummary!E8&lt;&gt;"",UnitSummary!E8,"")</f>
         <v>9</v>
       </c>
-      <c r="F5" s="2" t="str">
+      <c r="F5" s="39" t="str">
         <f>IF(UnitSummary!F8&lt;&gt;"",UnitSummary!F8,"")</f>
         <v/>
       </c>
-      <c r="G5" s="2" t="str">
+      <c r="G5" s="39" t="str">
         <f>IF(UnitSummary!G8&lt;&gt;"",UnitSummary!G8,"")</f>
         <v/>
       </c>
-      <c r="H5" s="2" t="str">
+      <c r="H5" s="39" t="str">
         <f>IF(UnitSummary!H8&lt;&gt;"",UnitSummary!H8,"")</f>
         <v/>
       </c>
-      <c r="I5" s="2" t="str">
+      <c r="I5" s="39" t="str">
         <f>IF(UnitSummary!I8&lt;&gt;"",UnitSummary!I8,"")</f>
         <v/>
       </c>
-      <c r="J5" s="2" t="str">
+      <c r="J5" s="39" t="str">
         <f>IF(UnitSummary!J8&lt;&gt;"",UnitSummary!J8,"")</f>
         <v/>
       </c>
-      <c r="K5" s="2" t="str">
+      <c r="K5" s="39" t="str">
         <f>IF(UnitSummary!K8&lt;&gt;"",UnitSummary!K8,"")</f>
         <v/>
       </c>
-      <c r="L5" s="2" t="str">
+      <c r="L5" s="39" t="str">
         <f>IF(UnitSummary!L8&lt;&gt;"",UnitSummary!L8,"")</f>
         <v/>
       </c>
-      <c r="M5" s="2" t="str">
+      <c r="M5" s="39" t="str">
         <f>IF(UnitSummary!M8&lt;&gt;"",UnitSummary!M8,"")</f>
         <v/>
       </c>
-      <c r="N5" s="2" t="str">
+      <c r="N5" s="39" t="str">
         <f>IF(UnitSummary!N8&lt;&gt;"",UnitSummary!N8,"")</f>
         <v/>
       </c>
-      <c r="O5" s="2" t="str">
+      <c r="O5" s="39" t="str">
         <f>IF(UnitSummary!O8&lt;&gt;"",UnitSummary!O8,"")</f>
         <v/>
       </c>
-      <c r="P5" s="2" t="str">
+      <c r="P5" s="39" t="str">
         <f>IF(UnitSummary!P8&lt;&gt;"",UnitSummary!P8,"")</f>
         <v/>
       </c>
-      <c r="Q5" s="2" t="str">
+      <c r="Q5" s="39" t="str">
         <f>IF(UnitSummary!Q8&lt;&gt;"",UnitSummary!Q8,"")</f>
         <v/>
       </c>
-      <c r="R5" s="2" t="str">
+      <c r="R5" s="39" t="str">
         <f>IF(UnitSummary!R8&lt;&gt;"",UnitSummary!R8,"")</f>
         <v/>
       </c>
-      <c r="S5" s="2" t="str">
+      <c r="S5" s="39" t="str">
         <f>IF(UnitSummary!S8&lt;&gt;"",UnitSummary!S8,"")</f>
         <v/>
       </c>
-      <c r="T5" s="2" t="str">
+      <c r="T5" s="39" t="str">
         <f>IF(UnitSummary!T8&lt;&gt;"",UnitSummary!T8,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="6" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="10"/>
+      <c r="V5" s="10"/>
+      <c r="W5" s="10"/>
+      <c r="X5" s="10"/>
+      <c r="Y5" s="10"/>
+      <c r="Z5" s="10"/>
+      <c r="AA5" s="10"/>
+      <c r="AB5" s="10"/>
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="10"/>
+      <c r="AE5" s="10"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="10"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="10"/>
+      <c r="AK5" s="10"/>
+      <c r="AL5" s="10"/>
+      <c r="AM5" s="10"/>
+      <c r="AN5" s="10"/>
+      <c r="AO5" s="10"/>
+      <c r="AP5" s="10"/>
+      <c r="AQ5" s="10"/>
+      <c r="AR5" s="10"/>
+      <c r="AS5" s="10"/>
+      <c r="AT5" s="10"/>
+      <c r="AU5" s="10"/>
+      <c r="AV5" s="10"/>
+      <c r="AW5" s="10"/>
+      <c r="AX5" s="10"/>
+      <c r="AY5" s="10"/>
+      <c r="AZ5" s="10"/>
+      <c r="BA5" s="10"/>
+      <c r="BB5" s="10"/>
+      <c r="BC5" s="10"/>
+      <c r="BD5" s="10"/>
+      <c r="BE5" s="10"/>
+      <c r="BF5" s="10"/>
+      <c r="BG5" s="10"/>
+      <c r="BH5" s="10"/>
+      <c r="BI5" s="10"/>
+      <c r="BJ5" s="10"/>
+      <c r="BK5" s="10"/>
+      <c r="BL5" s="10"/>
+      <c r="BM5" s="10"/>
+      <c r="BN5" s="10"/>
+      <c r="BO5" s="10"/>
+      <c r="BP5" s="10"/>
+      <c r="BQ5" s="10"/>
+      <c r="BR5" s="10"/>
+      <c r="BS5" s="10"/>
+      <c r="BT5" s="10"/>
+      <c r="BU5" s="10"/>
+      <c r="BV5" s="10"/>
+      <c r="BW5" s="10"/>
+      <c r="BX5" s="10"/>
+      <c r="BY5" s="10"/>
+      <c r="BZ5" s="10"/>
+      <c r="CA5" s="10"/>
+      <c r="CB5" s="10"/>
+      <c r="CC5" s="10"/>
+      <c r="CD5" s="10"/>
+    </row>
+    <row r="6" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="str">
         <f>IF(UnitSummary!A9&lt;&gt;"",UnitSummary!A9,"")</f>
         <v/>
@@ -1100,90 +1196,214 @@
         <f>IF(UnitSummary!T9&lt;&gt;"",UnitSummary!T9,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="7" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="str">
+      <c r="U6" s="10"/>
+      <c r="V6" s="10"/>
+      <c r="W6" s="10"/>
+      <c r="X6" s="10"/>
+      <c r="Y6" s="10"/>
+      <c r="Z6" s="10"/>
+      <c r="AA6" s="10"/>
+      <c r="AB6" s="10"/>
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="10"/>
+      <c r="AE6" s="10"/>
+      <c r="AF6" s="10"/>
+      <c r="AG6" s="10"/>
+      <c r="AH6" s="10"/>
+      <c r="AI6" s="10"/>
+      <c r="AJ6" s="10"/>
+      <c r="AK6" s="10"/>
+      <c r="AL6" s="10"/>
+      <c r="AM6" s="10"/>
+      <c r="AN6" s="10"/>
+      <c r="AO6" s="10"/>
+      <c r="AP6" s="10"/>
+      <c r="AQ6" s="10"/>
+      <c r="AR6" s="10"/>
+      <c r="AS6" s="10"/>
+      <c r="AT6" s="10"/>
+      <c r="AU6" s="10"/>
+      <c r="AV6" s="10"/>
+      <c r="AW6" s="10"/>
+      <c r="AX6" s="10"/>
+      <c r="AY6" s="10"/>
+      <c r="AZ6" s="10"/>
+      <c r="BA6" s="10"/>
+      <c r="BB6" s="10"/>
+      <c r="BC6" s="10"/>
+      <c r="BD6" s="10"/>
+      <c r="BE6" s="10"/>
+      <c r="BF6" s="10"/>
+      <c r="BG6" s="10"/>
+      <c r="BH6" s="10"/>
+      <c r="BI6" s="10"/>
+      <c r="BJ6" s="10"/>
+      <c r="BK6" s="10"/>
+      <c r="BL6" s="10"/>
+      <c r="BM6" s="10"/>
+      <c r="BN6" s="10"/>
+      <c r="BO6" s="10"/>
+      <c r="BP6" s="10"/>
+      <c r="BQ6" s="10"/>
+      <c r="BR6" s="10"/>
+      <c r="BS6" s="10"/>
+      <c r="BT6" s="10"/>
+      <c r="BU6" s="10"/>
+      <c r="BV6" s="10"/>
+      <c r="BW6" s="10"/>
+      <c r="BX6" s="10"/>
+      <c r="BY6" s="10"/>
+      <c r="BZ6" s="10"/>
+      <c r="CA6" s="10"/>
+      <c r="CB6" s="10"/>
+      <c r="CC6" s="10"/>
+      <c r="CD6" s="10"/>
+    </row>
+    <row r="7" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="39" t="str">
         <f>IF(UnitSummary!A10&lt;&gt;"",UnitSummary!A10,"")</f>
         <v/>
       </c>
-      <c r="B7" s="2" t="str">
+      <c r="B7" s="39" t="str">
         <f>IF(UnitSummary!B10&lt;&gt;"",UnitSummary!B10,"")</f>
         <v/>
       </c>
-      <c r="C7" s="2" t="str">
+      <c r="C7" s="39" t="str">
         <f>IF(UnitSummary!C10&lt;&gt;"",UnitSummary!C10,"")</f>
         <v/>
       </c>
-      <c r="D7" s="2" t="str">
+      <c r="D7" s="39" t="str">
         <f>IF(UnitSummary!D10&lt;&gt;"",UnitSummary!D10,"")</f>
         <v/>
       </c>
-      <c r="E7" s="2" t="str">
+      <c r="E7" s="39" t="str">
         <f>IF(UnitSummary!E10&lt;&gt;"",UnitSummary!E10,"")</f>
         <v/>
       </c>
-      <c r="F7" s="2" t="str">
+      <c r="F7" s="39" t="str">
         <f>IF(UnitSummary!F10&lt;&gt;"",UnitSummary!F10,"")</f>
         <v/>
       </c>
-      <c r="G7" s="2" t="str">
+      <c r="G7" s="39" t="str">
         <f>IF(UnitSummary!G10&lt;&gt;"",UnitSummary!G10,"")</f>
         <v/>
       </c>
-      <c r="H7" s="2" t="str">
+      <c r="H7" s="39" t="str">
         <f>IF(UnitSummary!H10&lt;&gt;"",UnitSummary!H10,"")</f>
         <v/>
       </c>
-      <c r="I7" s="2" t="str">
+      <c r="I7" s="39" t="str">
         <f>IF(UnitSummary!I10&lt;&gt;"",UnitSummary!I10,"")</f>
         <v/>
       </c>
-      <c r="J7" s="2" t="str">
+      <c r="J7" s="39" t="str">
         <f>IF(UnitSummary!J10&lt;&gt;"",UnitSummary!J10,"")</f>
         <v/>
       </c>
-      <c r="K7" s="2" t="str">
+      <c r="K7" s="39" t="str">
         <f>IF(UnitSummary!K10&lt;&gt;"",UnitSummary!K10,"")</f>
         <v/>
       </c>
-      <c r="L7" s="2" t="str">
+      <c r="L7" s="39" t="str">
         <f>IF(UnitSummary!L10&lt;&gt;"",UnitSummary!L10,"")</f>
         <v/>
       </c>
-      <c r="M7" s="2" t="str">
+      <c r="M7" s="39" t="str">
         <f>IF(UnitSummary!M10&lt;&gt;"",UnitSummary!M10,"")</f>
         <v/>
       </c>
-      <c r="N7" s="2" t="str">
+      <c r="N7" s="39" t="str">
         <f>IF(UnitSummary!N10&lt;&gt;"",UnitSummary!N10,"")</f>
         <v/>
       </c>
-      <c r="O7" s="2" t="str">
+      <c r="O7" s="39" t="str">
         <f>IF(UnitSummary!O10&lt;&gt;"",UnitSummary!O10,"")</f>
         <v/>
       </c>
-      <c r="P7" s="2" t="str">
+      <c r="P7" s="39" t="str">
         <f>IF(UnitSummary!P10&lt;&gt;"",UnitSummary!P10,"")</f>
         <v/>
       </c>
-      <c r="Q7" s="2" t="str">
+      <c r="Q7" s="39" t="str">
         <f>IF(UnitSummary!Q10&lt;&gt;"",UnitSummary!Q10,"")</f>
         <v/>
       </c>
-      <c r="R7" s="2" t="str">
+      <c r="R7" s="39" t="str">
         <f>IF(UnitSummary!R10&lt;&gt;"",UnitSummary!R10,"")</f>
         <v/>
       </c>
-      <c r="S7" s="2" t="str">
+      <c r="S7" s="39" t="str">
         <f>IF(UnitSummary!S10&lt;&gt;"",UnitSummary!S10,"")</f>
         <v/>
       </c>
-      <c r="T7" s="2" t="str">
+      <c r="T7" s="39" t="str">
         <f>IF(UnitSummary!T10&lt;&gt;"",UnitSummary!T10,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="8" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="10"/>
+      <c r="V7" s="10"/>
+      <c r="W7" s="10"/>
+      <c r="X7" s="10"/>
+      <c r="Y7" s="10"/>
+      <c r="Z7" s="10"/>
+      <c r="AA7" s="10"/>
+      <c r="AB7" s="10"/>
+      <c r="AC7" s="10"/>
+      <c r="AD7" s="10"/>
+      <c r="AE7" s="10"/>
+      <c r="AF7" s="10"/>
+      <c r="AG7" s="10"/>
+      <c r="AH7" s="10"/>
+      <c r="AI7" s="10"/>
+      <c r="AJ7" s="10"/>
+      <c r="AK7" s="10"/>
+      <c r="AL7" s="10"/>
+      <c r="AM7" s="10"/>
+      <c r="AN7" s="10"/>
+      <c r="AO7" s="10"/>
+      <c r="AP7" s="10"/>
+      <c r="AQ7" s="10"/>
+      <c r="AR7" s="10"/>
+      <c r="AS7" s="10"/>
+      <c r="AT7" s="10"/>
+      <c r="AU7" s="10"/>
+      <c r="AV7" s="10"/>
+      <c r="AW7" s="10"/>
+      <c r="AX7" s="10"/>
+      <c r="AY7" s="10"/>
+      <c r="AZ7" s="10"/>
+      <c r="BA7" s="10"/>
+      <c r="BB7" s="10"/>
+      <c r="BC7" s="10"/>
+      <c r="BD7" s="10"/>
+      <c r="BE7" s="10"/>
+      <c r="BF7" s="10"/>
+      <c r="BG7" s="10"/>
+      <c r="BH7" s="10"/>
+      <c r="BI7" s="10"/>
+      <c r="BJ7" s="10"/>
+      <c r="BK7" s="10"/>
+      <c r="BL7" s="10"/>
+      <c r="BM7" s="10"/>
+      <c r="BN7" s="10"/>
+      <c r="BO7" s="10"/>
+      <c r="BP7" s="10"/>
+      <c r="BQ7" s="10"/>
+      <c r="BR7" s="10"/>
+      <c r="BS7" s="10"/>
+      <c r="BT7" s="10"/>
+      <c r="BU7" s="10"/>
+      <c r="BV7" s="10"/>
+      <c r="BW7" s="10"/>
+      <c r="BX7" s="10"/>
+      <c r="BY7" s="10"/>
+      <c r="BZ7" s="10"/>
+      <c r="CA7" s="10"/>
+      <c r="CB7" s="10"/>
+      <c r="CC7" s="10"/>
+      <c r="CD7" s="10"/>
+    </row>
+    <row r="8" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="str">
         <f>IF(UnitSummary!A11&lt;&gt;"",UnitSummary!A11,"")</f>
         <v/>
@@ -1264,90 +1484,214 @@
         <f>IF(UnitSummary!T11&lt;&gt;"",UnitSummary!T11,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="9" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="str">
+      <c r="U8" s="10"/>
+      <c r="V8" s="10"/>
+      <c r="W8" s="10"/>
+      <c r="X8" s="10"/>
+      <c r="Y8" s="10"/>
+      <c r="Z8" s="10"/>
+      <c r="AA8" s="10"/>
+      <c r="AB8" s="10"/>
+      <c r="AC8" s="10"/>
+      <c r="AD8" s="10"/>
+      <c r="AE8" s="10"/>
+      <c r="AF8" s="10"/>
+      <c r="AG8" s="10"/>
+      <c r="AH8" s="10"/>
+      <c r="AI8" s="10"/>
+      <c r="AJ8" s="10"/>
+      <c r="AK8" s="10"/>
+      <c r="AL8" s="10"/>
+      <c r="AM8" s="10"/>
+      <c r="AN8" s="10"/>
+      <c r="AO8" s="10"/>
+      <c r="AP8" s="10"/>
+      <c r="AQ8" s="10"/>
+      <c r="AR8" s="10"/>
+      <c r="AS8" s="10"/>
+      <c r="AT8" s="10"/>
+      <c r="AU8" s="10"/>
+      <c r="AV8" s="10"/>
+      <c r="AW8" s="10"/>
+      <c r="AX8" s="10"/>
+      <c r="AY8" s="10"/>
+      <c r="AZ8" s="10"/>
+      <c r="BA8" s="10"/>
+      <c r="BB8" s="10"/>
+      <c r="BC8" s="10"/>
+      <c r="BD8" s="10"/>
+      <c r="BE8" s="10"/>
+      <c r="BF8" s="10"/>
+      <c r="BG8" s="10"/>
+      <c r="BH8" s="10"/>
+      <c r="BI8" s="10"/>
+      <c r="BJ8" s="10"/>
+      <c r="BK8" s="10"/>
+      <c r="BL8" s="10"/>
+      <c r="BM8" s="10"/>
+      <c r="BN8" s="10"/>
+      <c r="BO8" s="10"/>
+      <c r="BP8" s="10"/>
+      <c r="BQ8" s="10"/>
+      <c r="BR8" s="10"/>
+      <c r="BS8" s="10"/>
+      <c r="BT8" s="10"/>
+      <c r="BU8" s="10"/>
+      <c r="BV8" s="10"/>
+      <c r="BW8" s="10"/>
+      <c r="BX8" s="10"/>
+      <c r="BY8" s="10"/>
+      <c r="BZ8" s="10"/>
+      <c r="CA8" s="10"/>
+      <c r="CB8" s="10"/>
+      <c r="CC8" s="10"/>
+      <c r="CD8" s="10"/>
+    </row>
+    <row r="9" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="39" t="str">
         <f>IF(UnitSummary!A12&lt;&gt;"",UnitSummary!A12,"")</f>
         <v/>
       </c>
-      <c r="B9" s="2" t="str">
+      <c r="B9" s="39" t="str">
         <f>IF(UnitSummary!B12&lt;&gt;"",UnitSummary!B12,"")</f>
         <v/>
       </c>
-      <c r="C9" s="2" t="str">
+      <c r="C9" s="39" t="str">
         <f>IF(UnitSummary!C12&lt;&gt;"",UnitSummary!C12,"")</f>
         <v/>
       </c>
-      <c r="D9" s="2" t="str">
+      <c r="D9" s="39" t="str">
         <f>IF(UnitSummary!D12&lt;&gt;"",UnitSummary!D12,"")</f>
         <v/>
       </c>
-      <c r="E9" s="2" t="str">
+      <c r="E9" s="39" t="str">
         <f>IF(UnitSummary!E12&lt;&gt;"",UnitSummary!E12,"")</f>
         <v/>
       </c>
-      <c r="F9" s="2" t="str">
+      <c r="F9" s="39" t="str">
         <f>IF(UnitSummary!F12&lt;&gt;"",UnitSummary!F12,"")</f>
         <v/>
       </c>
-      <c r="G9" s="2" t="str">
+      <c r="G9" s="39" t="str">
         <f>IF(UnitSummary!G12&lt;&gt;"",UnitSummary!G12,"")</f>
         <v/>
       </c>
-      <c r="H9" s="2" t="str">
+      <c r="H9" s="39" t="str">
         <f>IF(UnitSummary!H12&lt;&gt;"",UnitSummary!H12,"")</f>
         <v/>
       </c>
-      <c r="I9" s="2" t="str">
+      <c r="I9" s="39" t="str">
         <f>IF(UnitSummary!I12&lt;&gt;"",UnitSummary!I12,"")</f>
         <v/>
       </c>
-      <c r="J9" s="2" t="str">
+      <c r="J9" s="39" t="str">
         <f>IF(UnitSummary!J12&lt;&gt;"",UnitSummary!J12,"")</f>
         <v/>
       </c>
-      <c r="K9" s="2" t="str">
+      <c r="K9" s="39" t="str">
         <f>IF(UnitSummary!K12&lt;&gt;"",UnitSummary!K12,"")</f>
         <v/>
       </c>
-      <c r="L9" s="2" t="str">
+      <c r="L9" s="39" t="str">
         <f>IF(UnitSummary!L12&lt;&gt;"",UnitSummary!L12,"")</f>
         <v/>
       </c>
-      <c r="M9" s="2" t="str">
+      <c r="M9" s="39" t="str">
         <f>IF(UnitSummary!M12&lt;&gt;"",UnitSummary!M12,"")</f>
         <v/>
       </c>
-      <c r="N9" s="2" t="str">
+      <c r="N9" s="39" t="str">
         <f>IF(UnitSummary!N12&lt;&gt;"",UnitSummary!N12,"")</f>
         <v/>
       </c>
-      <c r="O9" s="2" t="str">
+      <c r="O9" s="39" t="str">
         <f>IF(UnitSummary!O12&lt;&gt;"",UnitSummary!O12,"")</f>
         <v/>
       </c>
-      <c r="P9" s="2" t="str">
+      <c r="P9" s="39" t="str">
         <f>IF(UnitSummary!P12&lt;&gt;"",UnitSummary!P12,"")</f>
         <v/>
       </c>
-      <c r="Q9" s="2" t="str">
+      <c r="Q9" s="39" t="str">
         <f>IF(UnitSummary!Q12&lt;&gt;"",UnitSummary!Q12,"")</f>
         <v/>
       </c>
-      <c r="R9" s="2" t="str">
+      <c r="R9" s="39" t="str">
         <f>IF(UnitSummary!R12&lt;&gt;"",UnitSummary!R12,"")</f>
         <v/>
       </c>
-      <c r="S9" s="2" t="str">
+      <c r="S9" s="39" t="str">
         <f>IF(UnitSummary!S12&lt;&gt;"",UnitSummary!S12,"")</f>
         <v/>
       </c>
-      <c r="T9" s="2" t="str">
+      <c r="T9" s="39" t="str">
         <f>IF(UnitSummary!T12&lt;&gt;"",UnitSummary!T12,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="10" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="10"/>
+      <c r="V9" s="10"/>
+      <c r="W9" s="10"/>
+      <c r="X9" s="10"/>
+      <c r="Y9" s="10"/>
+      <c r="Z9" s="10"/>
+      <c r="AA9" s="10"/>
+      <c r="AB9" s="10"/>
+      <c r="AC9" s="10"/>
+      <c r="AD9" s="10"/>
+      <c r="AE9" s="10"/>
+      <c r="AF9" s="10"/>
+      <c r="AG9" s="10"/>
+      <c r="AH9" s="10"/>
+      <c r="AI9" s="10"/>
+      <c r="AJ9" s="10"/>
+      <c r="AK9" s="10"/>
+      <c r="AL9" s="10"/>
+      <c r="AM9" s="10"/>
+      <c r="AN9" s="10"/>
+      <c r="AO9" s="10"/>
+      <c r="AP9" s="10"/>
+      <c r="AQ9" s="10"/>
+      <c r="AR9" s="10"/>
+      <c r="AS9" s="10"/>
+      <c r="AT9" s="10"/>
+      <c r="AU9" s="10"/>
+      <c r="AV9" s="10"/>
+      <c r="AW9" s="10"/>
+      <c r="AX9" s="10"/>
+      <c r="AY9" s="10"/>
+      <c r="AZ9" s="10"/>
+      <c r="BA9" s="10"/>
+      <c r="BB9" s="10"/>
+      <c r="BC9" s="10"/>
+      <c r="BD9" s="10"/>
+      <c r="BE9" s="10"/>
+      <c r="BF9" s="10"/>
+      <c r="BG9" s="10"/>
+      <c r="BH9" s="10"/>
+      <c r="BI9" s="10"/>
+      <c r="BJ9" s="10"/>
+      <c r="BK9" s="10"/>
+      <c r="BL9" s="10"/>
+      <c r="BM9" s="10"/>
+      <c r="BN9" s="10"/>
+      <c r="BO9" s="10"/>
+      <c r="BP9" s="10"/>
+      <c r="BQ9" s="10"/>
+      <c r="BR9" s="10"/>
+      <c r="BS9" s="10"/>
+      <c r="BT9" s="10"/>
+      <c r="BU9" s="10"/>
+      <c r="BV9" s="10"/>
+      <c r="BW9" s="10"/>
+      <c r="BX9" s="10"/>
+      <c r="BY9" s="10"/>
+      <c r="BZ9" s="10"/>
+      <c r="CA9" s="10"/>
+      <c r="CB9" s="10"/>
+      <c r="CC9" s="10"/>
+      <c r="CD9" s="10"/>
+    </row>
+    <row r="10" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="str">
         <f>IF(UnitSummary!A13&lt;&gt;"",UnitSummary!A13,"")</f>
         <v/>
@@ -1428,90 +1772,214 @@
         <f>IF(UnitSummary!T13&lt;&gt;"",UnitSummary!T13,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="11" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="str">
+      <c r="U10" s="10"/>
+      <c r="V10" s="10"/>
+      <c r="W10" s="10"/>
+      <c r="X10" s="10"/>
+      <c r="Y10" s="10"/>
+      <c r="Z10" s="10"/>
+      <c r="AA10" s="10"/>
+      <c r="AB10" s="10"/>
+      <c r="AC10" s="10"/>
+      <c r="AD10" s="10"/>
+      <c r="AE10" s="10"/>
+      <c r="AF10" s="10"/>
+      <c r="AG10" s="10"/>
+      <c r="AH10" s="10"/>
+      <c r="AI10" s="10"/>
+      <c r="AJ10" s="10"/>
+      <c r="AK10" s="10"/>
+      <c r="AL10" s="10"/>
+      <c r="AM10" s="10"/>
+      <c r="AN10" s="10"/>
+      <c r="AO10" s="10"/>
+      <c r="AP10" s="10"/>
+      <c r="AQ10" s="10"/>
+      <c r="AR10" s="10"/>
+      <c r="AS10" s="10"/>
+      <c r="AT10" s="10"/>
+      <c r="AU10" s="10"/>
+      <c r="AV10" s="10"/>
+      <c r="AW10" s="10"/>
+      <c r="AX10" s="10"/>
+      <c r="AY10" s="10"/>
+      <c r="AZ10" s="10"/>
+      <c r="BA10" s="10"/>
+      <c r="BB10" s="10"/>
+      <c r="BC10" s="10"/>
+      <c r="BD10" s="10"/>
+      <c r="BE10" s="10"/>
+      <c r="BF10" s="10"/>
+      <c r="BG10" s="10"/>
+      <c r="BH10" s="10"/>
+      <c r="BI10" s="10"/>
+      <c r="BJ10" s="10"/>
+      <c r="BK10" s="10"/>
+      <c r="BL10" s="10"/>
+      <c r="BM10" s="10"/>
+      <c r="BN10" s="10"/>
+      <c r="BO10" s="10"/>
+      <c r="BP10" s="10"/>
+      <c r="BQ10" s="10"/>
+      <c r="BR10" s="10"/>
+      <c r="BS10" s="10"/>
+      <c r="BT10" s="10"/>
+      <c r="BU10" s="10"/>
+      <c r="BV10" s="10"/>
+      <c r="BW10" s="10"/>
+      <c r="BX10" s="10"/>
+      <c r="BY10" s="10"/>
+      <c r="BZ10" s="10"/>
+      <c r="CA10" s="10"/>
+      <c r="CB10" s="10"/>
+      <c r="CC10" s="10"/>
+      <c r="CD10" s="10"/>
+    </row>
+    <row r="11" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="39" t="str">
         <f>IF(UnitSummary!A14&lt;&gt;"",UnitSummary!A14,"")</f>
         <v/>
       </c>
-      <c r="B11" s="2" t="str">
+      <c r="B11" s="39" t="str">
         <f>IF(UnitSummary!B14&lt;&gt;"",UnitSummary!B14,"")</f>
         <v/>
       </c>
-      <c r="C11" s="2" t="str">
+      <c r="C11" s="39" t="str">
         <f>IF(UnitSummary!C14&lt;&gt;"",UnitSummary!C14,"")</f>
         <v/>
       </c>
-      <c r="D11" s="2" t="str">
+      <c r="D11" s="39" t="str">
         <f>IF(UnitSummary!D14&lt;&gt;"",UnitSummary!D14,"")</f>
         <v/>
       </c>
-      <c r="E11" s="2" t="str">
+      <c r="E11" s="39" t="str">
         <f>IF(UnitSummary!E14&lt;&gt;"",UnitSummary!E14,"")</f>
         <v/>
       </c>
-      <c r="F11" s="2" t="str">
+      <c r="F11" s="39" t="str">
         <f>IF(UnitSummary!F14&lt;&gt;"",UnitSummary!F14,"")</f>
         <v/>
       </c>
-      <c r="G11" s="2" t="str">
+      <c r="G11" s="39" t="str">
         <f>IF(UnitSummary!G14&lt;&gt;"",UnitSummary!G14,"")</f>
         <v/>
       </c>
-      <c r="H11" s="2" t="str">
+      <c r="H11" s="39" t="str">
         <f>IF(UnitSummary!H14&lt;&gt;"",UnitSummary!H14,"")</f>
         <v/>
       </c>
-      <c r="I11" s="2" t="str">
+      <c r="I11" s="39" t="str">
         <f>IF(UnitSummary!I14&lt;&gt;"",UnitSummary!I14,"")</f>
         <v/>
       </c>
-      <c r="J11" s="2" t="str">
+      <c r="J11" s="39" t="str">
         <f>IF(UnitSummary!J14&lt;&gt;"",UnitSummary!J14,"")</f>
         <v/>
       </c>
-      <c r="K11" s="2" t="str">
+      <c r="K11" s="39" t="str">
         <f>IF(UnitSummary!K14&lt;&gt;"",UnitSummary!K14,"")</f>
         <v/>
       </c>
-      <c r="L11" s="2" t="str">
+      <c r="L11" s="39" t="str">
         <f>IF(UnitSummary!L14&lt;&gt;"",UnitSummary!L14,"")</f>
         <v/>
       </c>
-      <c r="M11" s="2" t="str">
+      <c r="M11" s="39" t="str">
         <f>IF(UnitSummary!M14&lt;&gt;"",UnitSummary!M14,"")</f>
         <v/>
       </c>
-      <c r="N11" s="2" t="str">
+      <c r="N11" s="39" t="str">
         <f>IF(UnitSummary!N14&lt;&gt;"",UnitSummary!N14,"")</f>
         <v/>
       </c>
-      <c r="O11" s="2" t="str">
+      <c r="O11" s="39" t="str">
         <f>IF(UnitSummary!O14&lt;&gt;"",UnitSummary!O14,"")</f>
         <v/>
       </c>
-      <c r="P11" s="2" t="str">
+      <c r="P11" s="39" t="str">
         <f>IF(UnitSummary!P14&lt;&gt;"",UnitSummary!P14,"")</f>
         <v/>
       </c>
-      <c r="Q11" s="2" t="str">
+      <c r="Q11" s="39" t="str">
         <f>IF(UnitSummary!Q14&lt;&gt;"",UnitSummary!Q14,"")</f>
         <v/>
       </c>
-      <c r="R11" s="2" t="str">
+      <c r="R11" s="39" t="str">
         <f>IF(UnitSummary!R14&lt;&gt;"",UnitSummary!R14,"")</f>
         <v/>
       </c>
-      <c r="S11" s="2" t="str">
+      <c r="S11" s="39" t="str">
         <f>IF(UnitSummary!S14&lt;&gt;"",UnitSummary!S14,"")</f>
         <v/>
       </c>
-      <c r="T11" s="2" t="str">
+      <c r="T11" s="39" t="str">
         <f>IF(UnitSummary!T14&lt;&gt;"",UnitSummary!T14,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="12" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="10"/>
+      <c r="V11" s="10"/>
+      <c r="W11" s="10"/>
+      <c r="X11" s="10"/>
+      <c r="Y11" s="10"/>
+      <c r="Z11" s="10"/>
+      <c r="AA11" s="10"/>
+      <c r="AB11" s="10"/>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="10"/>
+      <c r="AE11" s="10"/>
+      <c r="AF11" s="10"/>
+      <c r="AG11" s="10"/>
+      <c r="AH11" s="10"/>
+      <c r="AI11" s="10"/>
+      <c r="AJ11" s="10"/>
+      <c r="AK11" s="10"/>
+      <c r="AL11" s="10"/>
+      <c r="AM11" s="10"/>
+      <c r="AN11" s="10"/>
+      <c r="AO11" s="10"/>
+      <c r="AP11" s="10"/>
+      <c r="AQ11" s="10"/>
+      <c r="AR11" s="10"/>
+      <c r="AS11" s="10"/>
+      <c r="AT11" s="10"/>
+      <c r="AU11" s="10"/>
+      <c r="AV11" s="10"/>
+      <c r="AW11" s="10"/>
+      <c r="AX11" s="10"/>
+      <c r="AY11" s="10"/>
+      <c r="AZ11" s="10"/>
+      <c r="BA11" s="10"/>
+      <c r="BB11" s="10"/>
+      <c r="BC11" s="10"/>
+      <c r="BD11" s="10"/>
+      <c r="BE11" s="10"/>
+      <c r="BF11" s="10"/>
+      <c r="BG11" s="10"/>
+      <c r="BH11" s="10"/>
+      <c r="BI11" s="10"/>
+      <c r="BJ11" s="10"/>
+      <c r="BK11" s="10"/>
+      <c r="BL11" s="10"/>
+      <c r="BM11" s="10"/>
+      <c r="BN11" s="10"/>
+      <c r="BO11" s="10"/>
+      <c r="BP11" s="10"/>
+      <c r="BQ11" s="10"/>
+      <c r="BR11" s="10"/>
+      <c r="BS11" s="10"/>
+      <c r="BT11" s="10"/>
+      <c r="BU11" s="10"/>
+      <c r="BV11" s="10"/>
+      <c r="BW11" s="10"/>
+      <c r="BX11" s="10"/>
+      <c r="BY11" s="10"/>
+      <c r="BZ11" s="10"/>
+      <c r="CA11" s="10"/>
+      <c r="CB11" s="10"/>
+      <c r="CC11" s="10"/>
+      <c r="CD11" s="10"/>
+    </row>
+    <row r="12" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="str">
         <f>IF(UnitSummary!A15&lt;&gt;"",UnitSummary!A15,"")</f>
         <v/>
@@ -1592,90 +2060,214 @@
         <f>IF(UnitSummary!T15&lt;&gt;"",UnitSummary!T15,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="13" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="str">
+      <c r="U12" s="10"/>
+      <c r="V12" s="10"/>
+      <c r="W12" s="10"/>
+      <c r="X12" s="10"/>
+      <c r="Y12" s="10"/>
+      <c r="Z12" s="10"/>
+      <c r="AA12" s="10"/>
+      <c r="AB12" s="10"/>
+      <c r="AC12" s="10"/>
+      <c r="AD12" s="10"/>
+      <c r="AE12" s="10"/>
+      <c r="AF12" s="10"/>
+      <c r="AG12" s="10"/>
+      <c r="AH12" s="10"/>
+      <c r="AI12" s="10"/>
+      <c r="AJ12" s="10"/>
+      <c r="AK12" s="10"/>
+      <c r="AL12" s="10"/>
+      <c r="AM12" s="10"/>
+      <c r="AN12" s="10"/>
+      <c r="AO12" s="10"/>
+      <c r="AP12" s="10"/>
+      <c r="AQ12" s="10"/>
+      <c r="AR12" s="10"/>
+      <c r="AS12" s="10"/>
+      <c r="AT12" s="10"/>
+      <c r="AU12" s="10"/>
+      <c r="AV12" s="10"/>
+      <c r="AW12" s="10"/>
+      <c r="AX12" s="10"/>
+      <c r="AY12" s="10"/>
+      <c r="AZ12" s="10"/>
+      <c r="BA12" s="10"/>
+      <c r="BB12" s="10"/>
+      <c r="BC12" s="10"/>
+      <c r="BD12" s="10"/>
+      <c r="BE12" s="10"/>
+      <c r="BF12" s="10"/>
+      <c r="BG12" s="10"/>
+      <c r="BH12" s="10"/>
+      <c r="BI12" s="10"/>
+      <c r="BJ12" s="10"/>
+      <c r="BK12" s="10"/>
+      <c r="BL12" s="10"/>
+      <c r="BM12" s="10"/>
+      <c r="BN12" s="10"/>
+      <c r="BO12" s="10"/>
+      <c r="BP12" s="10"/>
+      <c r="BQ12" s="10"/>
+      <c r="BR12" s="10"/>
+      <c r="BS12" s="10"/>
+      <c r="BT12" s="10"/>
+      <c r="BU12" s="10"/>
+      <c r="BV12" s="10"/>
+      <c r="BW12" s="10"/>
+      <c r="BX12" s="10"/>
+      <c r="BY12" s="10"/>
+      <c r="BZ12" s="10"/>
+      <c r="CA12" s="10"/>
+      <c r="CB12" s="10"/>
+      <c r="CC12" s="10"/>
+      <c r="CD12" s="10"/>
+    </row>
+    <row r="13" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="39" t="str">
         <f>IF(UnitSummary!A16&lt;&gt;"",UnitSummary!A16,"")</f>
         <v/>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B13" s="39" t="str">
         <f>IF(UnitSummary!B16&lt;&gt;"",UnitSummary!B16,"")</f>
         <v/>
       </c>
-      <c r="C13" s="2" t="str">
+      <c r="C13" s="39" t="str">
         <f>IF(UnitSummary!C16&lt;&gt;"",UnitSummary!C16,"")</f>
         <v/>
       </c>
-      <c r="D13" s="2" t="str">
+      <c r="D13" s="39" t="str">
         <f>IF(UnitSummary!D16&lt;&gt;"",UnitSummary!D16,"")</f>
         <v/>
       </c>
-      <c r="E13" s="2" t="str">
+      <c r="E13" s="39" t="str">
         <f>IF(UnitSummary!E16&lt;&gt;"",UnitSummary!E16,"")</f>
         <v/>
       </c>
-      <c r="F13" s="2" t="str">
+      <c r="F13" s="39" t="str">
         <f>IF(UnitSummary!F16&lt;&gt;"",UnitSummary!F16,"")</f>
         <v/>
       </c>
-      <c r="G13" s="2" t="str">
+      <c r="G13" s="39" t="str">
         <f>IF(UnitSummary!G16&lt;&gt;"",UnitSummary!G16,"")</f>
         <v/>
       </c>
-      <c r="H13" s="2" t="str">
+      <c r="H13" s="39" t="str">
         <f>IF(UnitSummary!H16&lt;&gt;"",UnitSummary!H16,"")</f>
         <v/>
       </c>
-      <c r="I13" s="2" t="str">
+      <c r="I13" s="39" t="str">
         <f>IF(UnitSummary!I16&lt;&gt;"",UnitSummary!I16,"")</f>
         <v/>
       </c>
-      <c r="J13" s="2" t="str">
+      <c r="J13" s="39" t="str">
         <f>IF(UnitSummary!J16&lt;&gt;"",UnitSummary!J16,"")</f>
         <v/>
       </c>
-      <c r="K13" s="2" t="str">
+      <c r="K13" s="39" t="str">
         <f>IF(UnitSummary!K16&lt;&gt;"",UnitSummary!K16,"")</f>
         <v/>
       </c>
-      <c r="L13" s="2" t="str">
+      <c r="L13" s="39" t="str">
         <f>IF(UnitSummary!L16&lt;&gt;"",UnitSummary!L16,"")</f>
         <v/>
       </c>
-      <c r="M13" s="2" t="str">
+      <c r="M13" s="39" t="str">
         <f>IF(UnitSummary!M16&lt;&gt;"",UnitSummary!M16,"")</f>
         <v/>
       </c>
-      <c r="N13" s="2" t="str">
+      <c r="N13" s="39" t="str">
         <f>IF(UnitSummary!N16&lt;&gt;"",UnitSummary!N16,"")</f>
         <v/>
       </c>
-      <c r="O13" s="2" t="str">
+      <c r="O13" s="39" t="str">
         <f>IF(UnitSummary!O16&lt;&gt;"",UnitSummary!O16,"")</f>
         <v/>
       </c>
-      <c r="P13" s="2" t="str">
+      <c r="P13" s="39" t="str">
         <f>IF(UnitSummary!P16&lt;&gt;"",UnitSummary!P16,"")</f>
         <v/>
       </c>
-      <c r="Q13" s="2" t="str">
+      <c r="Q13" s="39" t="str">
         <f>IF(UnitSummary!Q16&lt;&gt;"",UnitSummary!Q16,"")</f>
         <v/>
       </c>
-      <c r="R13" s="2" t="str">
+      <c r="R13" s="39" t="str">
         <f>IF(UnitSummary!R16&lt;&gt;"",UnitSummary!R16,"")</f>
         <v/>
       </c>
-      <c r="S13" s="2" t="str">
+      <c r="S13" s="39" t="str">
         <f>IF(UnitSummary!S16&lt;&gt;"",UnitSummary!S16,"")</f>
         <v/>
       </c>
-      <c r="T13" s="2" t="str">
+      <c r="T13" s="39" t="str">
         <f>IF(UnitSummary!T16&lt;&gt;"",UnitSummary!T16,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="14" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="10"/>
+      <c r="V13" s="10"/>
+      <c r="W13" s="10"/>
+      <c r="X13" s="10"/>
+      <c r="Y13" s="10"/>
+      <c r="Z13" s="10"/>
+      <c r="AA13" s="10"/>
+      <c r="AB13" s="10"/>
+      <c r="AC13" s="10"/>
+      <c r="AD13" s="10"/>
+      <c r="AE13" s="10"/>
+      <c r="AF13" s="10"/>
+      <c r="AG13" s="10"/>
+      <c r="AH13" s="10"/>
+      <c r="AI13" s="10"/>
+      <c r="AJ13" s="10"/>
+      <c r="AK13" s="10"/>
+      <c r="AL13" s="10"/>
+      <c r="AM13" s="10"/>
+      <c r="AN13" s="10"/>
+      <c r="AO13" s="10"/>
+      <c r="AP13" s="10"/>
+      <c r="AQ13" s="10"/>
+      <c r="AR13" s="10"/>
+      <c r="AS13" s="10"/>
+      <c r="AT13" s="10"/>
+      <c r="AU13" s="10"/>
+      <c r="AV13" s="10"/>
+      <c r="AW13" s="10"/>
+      <c r="AX13" s="10"/>
+      <c r="AY13" s="10"/>
+      <c r="AZ13" s="10"/>
+      <c r="BA13" s="10"/>
+      <c r="BB13" s="10"/>
+      <c r="BC13" s="10"/>
+      <c r="BD13" s="10"/>
+      <c r="BE13" s="10"/>
+      <c r="BF13" s="10"/>
+      <c r="BG13" s="10"/>
+      <c r="BH13" s="10"/>
+      <c r="BI13" s="10"/>
+      <c r="BJ13" s="10"/>
+      <c r="BK13" s="10"/>
+      <c r="BL13" s="10"/>
+      <c r="BM13" s="10"/>
+      <c r="BN13" s="10"/>
+      <c r="BO13" s="10"/>
+      <c r="BP13" s="10"/>
+      <c r="BQ13" s="10"/>
+      <c r="BR13" s="10"/>
+      <c r="BS13" s="10"/>
+      <c r="BT13" s="10"/>
+      <c r="BU13" s="10"/>
+      <c r="BV13" s="10"/>
+      <c r="BW13" s="10"/>
+      <c r="BX13" s="10"/>
+      <c r="BY13" s="10"/>
+      <c r="BZ13" s="10"/>
+      <c r="CA13" s="10"/>
+      <c r="CB13" s="10"/>
+      <c r="CC13" s="10"/>
+      <c r="CD13" s="10"/>
+    </row>
+    <row r="14" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="str">
         <f>IF(UnitSummary!A17&lt;&gt;"",UnitSummary!A17,"")</f>
         <v/>
@@ -1756,90 +2348,214 @@
         <f>IF(UnitSummary!T17&lt;&gt;"",UnitSummary!T17,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="15" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="str">
+      <c r="U14" s="10"/>
+      <c r="V14" s="10"/>
+      <c r="W14" s="10"/>
+      <c r="X14" s="10"/>
+      <c r="Y14" s="10"/>
+      <c r="Z14" s="10"/>
+      <c r="AA14" s="10"/>
+      <c r="AB14" s="10"/>
+      <c r="AC14" s="10"/>
+      <c r="AD14" s="10"/>
+      <c r="AE14" s="10"/>
+      <c r="AF14" s="10"/>
+      <c r="AG14" s="10"/>
+      <c r="AH14" s="10"/>
+      <c r="AI14" s="10"/>
+      <c r="AJ14" s="10"/>
+      <c r="AK14" s="10"/>
+      <c r="AL14" s="10"/>
+      <c r="AM14" s="10"/>
+      <c r="AN14" s="10"/>
+      <c r="AO14" s="10"/>
+      <c r="AP14" s="10"/>
+      <c r="AQ14" s="10"/>
+      <c r="AR14" s="10"/>
+      <c r="AS14" s="10"/>
+      <c r="AT14" s="10"/>
+      <c r="AU14" s="10"/>
+      <c r="AV14" s="10"/>
+      <c r="AW14" s="10"/>
+      <c r="AX14" s="10"/>
+      <c r="AY14" s="10"/>
+      <c r="AZ14" s="10"/>
+      <c r="BA14" s="10"/>
+      <c r="BB14" s="10"/>
+      <c r="BC14" s="10"/>
+      <c r="BD14" s="10"/>
+      <c r="BE14" s="10"/>
+      <c r="BF14" s="10"/>
+      <c r="BG14" s="10"/>
+      <c r="BH14" s="10"/>
+      <c r="BI14" s="10"/>
+      <c r="BJ14" s="10"/>
+      <c r="BK14" s="10"/>
+      <c r="BL14" s="10"/>
+      <c r="BM14" s="10"/>
+      <c r="BN14" s="10"/>
+      <c r="BO14" s="10"/>
+      <c r="BP14" s="10"/>
+      <c r="BQ14" s="10"/>
+      <c r="BR14" s="10"/>
+      <c r="BS14" s="10"/>
+      <c r="BT14" s="10"/>
+      <c r="BU14" s="10"/>
+      <c r="BV14" s="10"/>
+      <c r="BW14" s="10"/>
+      <c r="BX14" s="10"/>
+      <c r="BY14" s="10"/>
+      <c r="BZ14" s="10"/>
+      <c r="CA14" s="10"/>
+      <c r="CB14" s="10"/>
+      <c r="CC14" s="10"/>
+      <c r="CD14" s="10"/>
+    </row>
+    <row r="15" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="39" t="str">
         <f>IF(UnitSummary!A18&lt;&gt;"",UnitSummary!A18,"")</f>
         <v/>
       </c>
-      <c r="B15" s="2" t="str">
+      <c r="B15" s="39" t="str">
         <f>IF(UnitSummary!B18&lt;&gt;"",UnitSummary!B18,"")</f>
         <v/>
       </c>
-      <c r="C15" s="2" t="str">
+      <c r="C15" s="39" t="str">
         <f>IF(UnitSummary!C18&lt;&gt;"",UnitSummary!C18,"")</f>
         <v/>
       </c>
-      <c r="D15" s="2" t="str">
+      <c r="D15" s="39" t="str">
         <f>IF(UnitSummary!D18&lt;&gt;"",UnitSummary!D18,"")</f>
         <v/>
       </c>
-      <c r="E15" s="2" t="str">
+      <c r="E15" s="39" t="str">
         <f>IF(UnitSummary!E18&lt;&gt;"",UnitSummary!E18,"")</f>
         <v/>
       </c>
-      <c r="F15" s="2" t="str">
+      <c r="F15" s="39" t="str">
         <f>IF(UnitSummary!F18&lt;&gt;"",UnitSummary!F18,"")</f>
         <v/>
       </c>
-      <c r="G15" s="2" t="str">
+      <c r="G15" s="39" t="str">
         <f>IF(UnitSummary!G18&lt;&gt;"",UnitSummary!G18,"")</f>
         <v/>
       </c>
-      <c r="H15" s="2" t="str">
+      <c r="H15" s="39" t="str">
         <f>IF(UnitSummary!H18&lt;&gt;"",UnitSummary!H18,"")</f>
         <v/>
       </c>
-      <c r="I15" s="2" t="str">
+      <c r="I15" s="39" t="str">
         <f>IF(UnitSummary!I18&lt;&gt;"",UnitSummary!I18,"")</f>
         <v/>
       </c>
-      <c r="J15" s="2" t="str">
+      <c r="J15" s="39" t="str">
         <f>IF(UnitSummary!J18&lt;&gt;"",UnitSummary!J18,"")</f>
         <v/>
       </c>
-      <c r="K15" s="2" t="str">
+      <c r="K15" s="39" t="str">
         <f>IF(UnitSummary!K18&lt;&gt;"",UnitSummary!K18,"")</f>
         <v/>
       </c>
-      <c r="L15" s="2" t="str">
+      <c r="L15" s="39" t="str">
         <f>IF(UnitSummary!L18&lt;&gt;"",UnitSummary!L18,"")</f>
         <v/>
       </c>
-      <c r="M15" s="2" t="str">
+      <c r="M15" s="39" t="str">
         <f>IF(UnitSummary!M18&lt;&gt;"",UnitSummary!M18,"")</f>
         <v/>
       </c>
-      <c r="N15" s="2" t="str">
+      <c r="N15" s="39" t="str">
         <f>IF(UnitSummary!N18&lt;&gt;"",UnitSummary!N18,"")</f>
         <v/>
       </c>
-      <c r="O15" s="2" t="str">
+      <c r="O15" s="39" t="str">
         <f>IF(UnitSummary!O18&lt;&gt;"",UnitSummary!O18,"")</f>
         <v/>
       </c>
-      <c r="P15" s="2" t="str">
+      <c r="P15" s="39" t="str">
         <f>IF(UnitSummary!P18&lt;&gt;"",UnitSummary!P18,"")</f>
         <v/>
       </c>
-      <c r="Q15" s="2" t="str">
+      <c r="Q15" s="39" t="str">
         <f>IF(UnitSummary!Q18&lt;&gt;"",UnitSummary!Q18,"")</f>
         <v/>
       </c>
-      <c r="R15" s="2" t="str">
+      <c r="R15" s="39" t="str">
         <f>IF(UnitSummary!R18&lt;&gt;"",UnitSummary!R18,"")</f>
         <v/>
       </c>
-      <c r="S15" s="2" t="str">
+      <c r="S15" s="39" t="str">
         <f>IF(UnitSummary!S18&lt;&gt;"",UnitSummary!S18,"")</f>
         <v/>
       </c>
-      <c r="T15" s="2" t="str">
+      <c r="T15" s="39" t="str">
         <f>IF(UnitSummary!T18&lt;&gt;"",UnitSummary!T18,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="16" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="10"/>
+      <c r="V15" s="10"/>
+      <c r="W15" s="10"/>
+      <c r="X15" s="10"/>
+      <c r="Y15" s="10"/>
+      <c r="Z15" s="10"/>
+      <c r="AA15" s="10"/>
+      <c r="AB15" s="10"/>
+      <c r="AC15" s="10"/>
+      <c r="AD15" s="10"/>
+      <c r="AE15" s="10"/>
+      <c r="AF15" s="10"/>
+      <c r="AG15" s="10"/>
+      <c r="AH15" s="10"/>
+      <c r="AI15" s="10"/>
+      <c r="AJ15" s="10"/>
+      <c r="AK15" s="10"/>
+      <c r="AL15" s="10"/>
+      <c r="AM15" s="10"/>
+      <c r="AN15" s="10"/>
+      <c r="AO15" s="10"/>
+      <c r="AP15" s="10"/>
+      <c r="AQ15" s="10"/>
+      <c r="AR15" s="10"/>
+      <c r="AS15" s="10"/>
+      <c r="AT15" s="10"/>
+      <c r="AU15" s="10"/>
+      <c r="AV15" s="10"/>
+      <c r="AW15" s="10"/>
+      <c r="AX15" s="10"/>
+      <c r="AY15" s="10"/>
+      <c r="AZ15" s="10"/>
+      <c r="BA15" s="10"/>
+      <c r="BB15" s="10"/>
+      <c r="BC15" s="10"/>
+      <c r="BD15" s="10"/>
+      <c r="BE15" s="10"/>
+      <c r="BF15" s="10"/>
+      <c r="BG15" s="10"/>
+      <c r="BH15" s="10"/>
+      <c r="BI15" s="10"/>
+      <c r="BJ15" s="10"/>
+      <c r="BK15" s="10"/>
+      <c r="BL15" s="10"/>
+      <c r="BM15" s="10"/>
+      <c r="BN15" s="10"/>
+      <c r="BO15" s="10"/>
+      <c r="BP15" s="10"/>
+      <c r="BQ15" s="10"/>
+      <c r="BR15" s="10"/>
+      <c r="BS15" s="10"/>
+      <c r="BT15" s="10"/>
+      <c r="BU15" s="10"/>
+      <c r="BV15" s="10"/>
+      <c r="BW15" s="10"/>
+      <c r="BX15" s="10"/>
+      <c r="BY15" s="10"/>
+      <c r="BZ15" s="10"/>
+      <c r="CA15" s="10"/>
+      <c r="CB15" s="10"/>
+      <c r="CC15" s="10"/>
+      <c r="CD15" s="10"/>
+    </row>
+    <row r="16" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="str">
         <f>IF(UnitSummary!A19&lt;&gt;"",UnitSummary!A19,"")</f>
         <v/>
@@ -1920,90 +2636,214 @@
         <f>IF(UnitSummary!T19&lt;&gt;"",UnitSummary!T19,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="17" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="str">
+      <c r="U16" s="10"/>
+      <c r="V16" s="10"/>
+      <c r="W16" s="10"/>
+      <c r="X16" s="10"/>
+      <c r="Y16" s="10"/>
+      <c r="Z16" s="10"/>
+      <c r="AA16" s="10"/>
+      <c r="AB16" s="10"/>
+      <c r="AC16" s="10"/>
+      <c r="AD16" s="10"/>
+      <c r="AE16" s="10"/>
+      <c r="AF16" s="10"/>
+      <c r="AG16" s="10"/>
+      <c r="AH16" s="10"/>
+      <c r="AI16" s="10"/>
+      <c r="AJ16" s="10"/>
+      <c r="AK16" s="10"/>
+      <c r="AL16" s="10"/>
+      <c r="AM16" s="10"/>
+      <c r="AN16" s="10"/>
+      <c r="AO16" s="10"/>
+      <c r="AP16" s="10"/>
+      <c r="AQ16" s="10"/>
+      <c r="AR16" s="10"/>
+      <c r="AS16" s="10"/>
+      <c r="AT16" s="10"/>
+      <c r="AU16" s="10"/>
+      <c r="AV16" s="10"/>
+      <c r="AW16" s="10"/>
+      <c r="AX16" s="10"/>
+      <c r="AY16" s="10"/>
+      <c r="AZ16" s="10"/>
+      <c r="BA16" s="10"/>
+      <c r="BB16" s="10"/>
+      <c r="BC16" s="10"/>
+      <c r="BD16" s="10"/>
+      <c r="BE16" s="10"/>
+      <c r="BF16" s="10"/>
+      <c r="BG16" s="10"/>
+      <c r="BH16" s="10"/>
+      <c r="BI16" s="10"/>
+      <c r="BJ16" s="10"/>
+      <c r="BK16" s="10"/>
+      <c r="BL16" s="10"/>
+      <c r="BM16" s="10"/>
+      <c r="BN16" s="10"/>
+      <c r="BO16" s="10"/>
+      <c r="BP16" s="10"/>
+      <c r="BQ16" s="10"/>
+      <c r="BR16" s="10"/>
+      <c r="BS16" s="10"/>
+      <c r="BT16" s="10"/>
+      <c r="BU16" s="10"/>
+      <c r="BV16" s="10"/>
+      <c r="BW16" s="10"/>
+      <c r="BX16" s="10"/>
+      <c r="BY16" s="10"/>
+      <c r="BZ16" s="10"/>
+      <c r="CA16" s="10"/>
+      <c r="CB16" s="10"/>
+      <c r="CC16" s="10"/>
+      <c r="CD16" s="10"/>
+    </row>
+    <row r="17" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="39" t="str">
         <f>IF(UnitSummary!A20&lt;&gt;"",UnitSummary!A20,"")</f>
         <v/>
       </c>
-      <c r="B17" s="2" t="str">
+      <c r="B17" s="39" t="str">
         <f>IF(UnitSummary!B20&lt;&gt;"",UnitSummary!B20,"")</f>
         <v/>
       </c>
-      <c r="C17" s="2" t="str">
+      <c r="C17" s="39" t="str">
         <f>IF(UnitSummary!C20&lt;&gt;"",UnitSummary!C20,"")</f>
         <v/>
       </c>
-      <c r="D17" s="2" t="str">
+      <c r="D17" s="39" t="str">
         <f>IF(UnitSummary!D20&lt;&gt;"",UnitSummary!D20,"")</f>
         <v/>
       </c>
-      <c r="E17" s="2" t="str">
+      <c r="E17" s="39" t="str">
         <f>IF(UnitSummary!E20&lt;&gt;"",UnitSummary!E20,"")</f>
         <v/>
       </c>
-      <c r="F17" s="2" t="str">
+      <c r="F17" s="39" t="str">
         <f>IF(UnitSummary!F20&lt;&gt;"",UnitSummary!F20,"")</f>
         <v/>
       </c>
-      <c r="G17" s="2" t="str">
+      <c r="G17" s="39" t="str">
         <f>IF(UnitSummary!G20&lt;&gt;"",UnitSummary!G20,"")</f>
         <v/>
       </c>
-      <c r="H17" s="2" t="str">
+      <c r="H17" s="39" t="str">
         <f>IF(UnitSummary!H20&lt;&gt;"",UnitSummary!H20,"")</f>
         <v/>
       </c>
-      <c r="I17" s="2" t="str">
+      <c r="I17" s="39" t="str">
         <f>IF(UnitSummary!I20&lt;&gt;"",UnitSummary!I20,"")</f>
         <v/>
       </c>
-      <c r="J17" s="2" t="str">
+      <c r="J17" s="39" t="str">
         <f>IF(UnitSummary!J20&lt;&gt;"",UnitSummary!J20,"")</f>
         <v/>
       </c>
-      <c r="K17" s="2" t="str">
+      <c r="K17" s="39" t="str">
         <f>IF(UnitSummary!K20&lt;&gt;"",UnitSummary!K20,"")</f>
         <v/>
       </c>
-      <c r="L17" s="2" t="str">
+      <c r="L17" s="39" t="str">
         <f>IF(UnitSummary!L20&lt;&gt;"",UnitSummary!L20,"")</f>
         <v/>
       </c>
-      <c r="M17" s="2" t="str">
+      <c r="M17" s="39" t="str">
         <f>IF(UnitSummary!M20&lt;&gt;"",UnitSummary!M20,"")</f>
         <v/>
       </c>
-      <c r="N17" s="2" t="str">
+      <c r="N17" s="39" t="str">
         <f>IF(UnitSummary!N20&lt;&gt;"",UnitSummary!N20,"")</f>
         <v/>
       </c>
-      <c r="O17" s="2" t="str">
+      <c r="O17" s="39" t="str">
         <f>IF(UnitSummary!O20&lt;&gt;"",UnitSummary!O20,"")</f>
         <v/>
       </c>
-      <c r="P17" s="2" t="str">
+      <c r="P17" s="39" t="str">
         <f>IF(UnitSummary!P20&lt;&gt;"",UnitSummary!P20,"")</f>
         <v/>
       </c>
-      <c r="Q17" s="2" t="str">
+      <c r="Q17" s="39" t="str">
         <f>IF(UnitSummary!Q20&lt;&gt;"",UnitSummary!Q20,"")</f>
         <v/>
       </c>
-      <c r="R17" s="2" t="str">
+      <c r="R17" s="39" t="str">
         <f>IF(UnitSummary!R20&lt;&gt;"",UnitSummary!R20,"")</f>
         <v/>
       </c>
-      <c r="S17" s="2" t="str">
+      <c r="S17" s="39" t="str">
         <f>IF(UnitSummary!S20&lt;&gt;"",UnitSummary!S20,"")</f>
         <v/>
       </c>
-      <c r="T17" s="2" t="str">
+      <c r="T17" s="39" t="str">
         <f>IF(UnitSummary!T20&lt;&gt;"",UnitSummary!T20,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="18" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="10"/>
+      <c r="V17" s="10"/>
+      <c r="W17" s="10"/>
+      <c r="X17" s="10"/>
+      <c r="Y17" s="10"/>
+      <c r="Z17" s="10"/>
+      <c r="AA17" s="10"/>
+      <c r="AB17" s="10"/>
+      <c r="AC17" s="10"/>
+      <c r="AD17" s="10"/>
+      <c r="AE17" s="10"/>
+      <c r="AF17" s="10"/>
+      <c r="AG17" s="10"/>
+      <c r="AH17" s="10"/>
+      <c r="AI17" s="10"/>
+      <c r="AJ17" s="10"/>
+      <c r="AK17" s="10"/>
+      <c r="AL17" s="10"/>
+      <c r="AM17" s="10"/>
+      <c r="AN17" s="10"/>
+      <c r="AO17" s="10"/>
+      <c r="AP17" s="10"/>
+      <c r="AQ17" s="10"/>
+      <c r="AR17" s="10"/>
+      <c r="AS17" s="10"/>
+      <c r="AT17" s="10"/>
+      <c r="AU17" s="10"/>
+      <c r="AV17" s="10"/>
+      <c r="AW17" s="10"/>
+      <c r="AX17" s="10"/>
+      <c r="AY17" s="10"/>
+      <c r="AZ17" s="10"/>
+      <c r="BA17" s="10"/>
+      <c r="BB17" s="10"/>
+      <c r="BC17" s="10"/>
+      <c r="BD17" s="10"/>
+      <c r="BE17" s="10"/>
+      <c r="BF17" s="10"/>
+      <c r="BG17" s="10"/>
+      <c r="BH17" s="10"/>
+      <c r="BI17" s="10"/>
+      <c r="BJ17" s="10"/>
+      <c r="BK17" s="10"/>
+      <c r="BL17" s="10"/>
+      <c r="BM17" s="10"/>
+      <c r="BN17" s="10"/>
+      <c r="BO17" s="10"/>
+      <c r="BP17" s="10"/>
+      <c r="BQ17" s="10"/>
+      <c r="BR17" s="10"/>
+      <c r="BS17" s="10"/>
+      <c r="BT17" s="10"/>
+      <c r="BU17" s="10"/>
+      <c r="BV17" s="10"/>
+      <c r="BW17" s="10"/>
+      <c r="BX17" s="10"/>
+      <c r="BY17" s="10"/>
+      <c r="BZ17" s="10"/>
+      <c r="CA17" s="10"/>
+      <c r="CB17" s="10"/>
+      <c r="CC17" s="10"/>
+      <c r="CD17" s="10"/>
+    </row>
+    <row r="18" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="str">
         <f>IF(UnitSummary!A21&lt;&gt;"",UnitSummary!A21,"")</f>
         <v/>
@@ -2084,90 +2924,214 @@
         <f>IF(UnitSummary!T21&lt;&gt;"",UnitSummary!T21,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="19" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2" t="str">
+      <c r="U18" s="10"/>
+      <c r="V18" s="10"/>
+      <c r="W18" s="10"/>
+      <c r="X18" s="10"/>
+      <c r="Y18" s="10"/>
+      <c r="Z18" s="10"/>
+      <c r="AA18" s="10"/>
+      <c r="AB18" s="10"/>
+      <c r="AC18" s="10"/>
+      <c r="AD18" s="10"/>
+      <c r="AE18" s="10"/>
+      <c r="AF18" s="10"/>
+      <c r="AG18" s="10"/>
+      <c r="AH18" s="10"/>
+      <c r="AI18" s="10"/>
+      <c r="AJ18" s="10"/>
+      <c r="AK18" s="10"/>
+      <c r="AL18" s="10"/>
+      <c r="AM18" s="10"/>
+      <c r="AN18" s="10"/>
+      <c r="AO18" s="10"/>
+      <c r="AP18" s="10"/>
+      <c r="AQ18" s="10"/>
+      <c r="AR18" s="10"/>
+      <c r="AS18" s="10"/>
+      <c r="AT18" s="10"/>
+      <c r="AU18" s="10"/>
+      <c r="AV18" s="10"/>
+      <c r="AW18" s="10"/>
+      <c r="AX18" s="10"/>
+      <c r="AY18" s="10"/>
+      <c r="AZ18" s="10"/>
+      <c r="BA18" s="10"/>
+      <c r="BB18" s="10"/>
+      <c r="BC18" s="10"/>
+      <c r="BD18" s="10"/>
+      <c r="BE18" s="10"/>
+      <c r="BF18" s="10"/>
+      <c r="BG18" s="10"/>
+      <c r="BH18" s="10"/>
+      <c r="BI18" s="10"/>
+      <c r="BJ18" s="10"/>
+      <c r="BK18" s="10"/>
+      <c r="BL18" s="10"/>
+      <c r="BM18" s="10"/>
+      <c r="BN18" s="10"/>
+      <c r="BO18" s="10"/>
+      <c r="BP18" s="10"/>
+      <c r="BQ18" s="10"/>
+      <c r="BR18" s="10"/>
+      <c r="BS18" s="10"/>
+      <c r="BT18" s="10"/>
+      <c r="BU18" s="10"/>
+      <c r="BV18" s="10"/>
+      <c r="BW18" s="10"/>
+      <c r="BX18" s="10"/>
+      <c r="BY18" s="10"/>
+      <c r="BZ18" s="10"/>
+      <c r="CA18" s="10"/>
+      <c r="CB18" s="10"/>
+      <c r="CC18" s="10"/>
+      <c r="CD18" s="10"/>
+    </row>
+    <row r="19" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="str">
         <f>IF(UnitSummary!A22&lt;&gt;"",UnitSummary!A22,"")</f>
         <v/>
       </c>
-      <c r="B19" s="2" t="str">
+      <c r="B19" s="39" t="str">
         <f>IF(UnitSummary!B22&lt;&gt;"",UnitSummary!B22,"")</f>
         <v/>
       </c>
-      <c r="C19" s="2" t="str">
+      <c r="C19" s="39" t="str">
         <f>IF(UnitSummary!C22&lt;&gt;"",UnitSummary!C22,"")</f>
         <v/>
       </c>
-      <c r="D19" s="2" t="str">
+      <c r="D19" s="39" t="str">
         <f>IF(UnitSummary!D22&lt;&gt;"",UnitSummary!D22,"")</f>
         <v/>
       </c>
-      <c r="E19" s="2" t="str">
+      <c r="E19" s="39" t="str">
         <f>IF(UnitSummary!E22&lt;&gt;"",UnitSummary!E22,"")</f>
         <v/>
       </c>
-      <c r="F19" s="2" t="str">
+      <c r="F19" s="39" t="str">
         <f>IF(UnitSummary!F22&lt;&gt;"",UnitSummary!F22,"")</f>
         <v/>
       </c>
-      <c r="G19" s="2" t="str">
+      <c r="G19" s="39" t="str">
         <f>IF(UnitSummary!G22&lt;&gt;"",UnitSummary!G22,"")</f>
         <v/>
       </c>
-      <c r="H19" s="2" t="str">
+      <c r="H19" s="39" t="str">
         <f>IF(UnitSummary!H22&lt;&gt;"",UnitSummary!H22,"")</f>
         <v/>
       </c>
-      <c r="I19" s="2" t="str">
+      <c r="I19" s="39" t="str">
         <f>IF(UnitSummary!I22&lt;&gt;"",UnitSummary!I22,"")</f>
         <v/>
       </c>
-      <c r="J19" s="2" t="str">
+      <c r="J19" s="39" t="str">
         <f>IF(UnitSummary!J22&lt;&gt;"",UnitSummary!J22,"")</f>
         <v/>
       </c>
-      <c r="K19" s="2" t="str">
+      <c r="K19" s="39" t="str">
         <f>IF(UnitSummary!K22&lt;&gt;"",UnitSummary!K22,"")</f>
         <v/>
       </c>
-      <c r="L19" s="2" t="str">
+      <c r="L19" s="39" t="str">
         <f>IF(UnitSummary!L22&lt;&gt;"",UnitSummary!L22,"")</f>
         <v/>
       </c>
-      <c r="M19" s="2" t="str">
+      <c r="M19" s="39" t="str">
         <f>IF(UnitSummary!M22&lt;&gt;"",UnitSummary!M22,"")</f>
         <v/>
       </c>
-      <c r="N19" s="2" t="str">
+      <c r="N19" s="39" t="str">
         <f>IF(UnitSummary!N22&lt;&gt;"",UnitSummary!N22,"")</f>
         <v/>
       </c>
-      <c r="O19" s="2" t="str">
+      <c r="O19" s="39" t="str">
         <f>IF(UnitSummary!O22&lt;&gt;"",UnitSummary!O22,"")</f>
         <v/>
       </c>
-      <c r="P19" s="2" t="str">
+      <c r="P19" s="39" t="str">
         <f>IF(UnitSummary!P22&lt;&gt;"",UnitSummary!P22,"")</f>
         <v/>
       </c>
-      <c r="Q19" s="2" t="str">
+      <c r="Q19" s="39" t="str">
         <f>IF(UnitSummary!Q22&lt;&gt;"",UnitSummary!Q22,"")</f>
         <v/>
       </c>
-      <c r="R19" s="2" t="str">
+      <c r="R19" s="39" t="str">
         <f>IF(UnitSummary!R22&lt;&gt;"",UnitSummary!R22,"")</f>
         <v/>
       </c>
-      <c r="S19" s="2" t="str">
+      <c r="S19" s="39" t="str">
         <f>IF(UnitSummary!S22&lt;&gt;"",UnitSummary!S22,"")</f>
         <v/>
       </c>
-      <c r="T19" s="2" t="str">
+      <c r="T19" s="39" t="str">
         <f>IF(UnitSummary!T22&lt;&gt;"",UnitSummary!T22,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="20" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="10"/>
+      <c r="V19" s="10"/>
+      <c r="W19" s="10"/>
+      <c r="X19" s="10"/>
+      <c r="Y19" s="10"/>
+      <c r="Z19" s="10"/>
+      <c r="AA19" s="10"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="10"/>
+      <c r="AD19" s="10"/>
+      <c r="AE19" s="10"/>
+      <c r="AF19" s="10"/>
+      <c r="AG19" s="10"/>
+      <c r="AH19" s="10"/>
+      <c r="AI19" s="10"/>
+      <c r="AJ19" s="10"/>
+      <c r="AK19" s="10"/>
+      <c r="AL19" s="10"/>
+      <c r="AM19" s="10"/>
+      <c r="AN19" s="10"/>
+      <c r="AO19" s="10"/>
+      <c r="AP19" s="10"/>
+      <c r="AQ19" s="10"/>
+      <c r="AR19" s="10"/>
+      <c r="AS19" s="10"/>
+      <c r="AT19" s="10"/>
+      <c r="AU19" s="10"/>
+      <c r="AV19" s="10"/>
+      <c r="AW19" s="10"/>
+      <c r="AX19" s="10"/>
+      <c r="AY19" s="10"/>
+      <c r="AZ19" s="10"/>
+      <c r="BA19" s="10"/>
+      <c r="BB19" s="10"/>
+      <c r="BC19" s="10"/>
+      <c r="BD19" s="10"/>
+      <c r="BE19" s="10"/>
+      <c r="BF19" s="10"/>
+      <c r="BG19" s="10"/>
+      <c r="BH19" s="10"/>
+      <c r="BI19" s="10"/>
+      <c r="BJ19" s="10"/>
+      <c r="BK19" s="10"/>
+      <c r="BL19" s="10"/>
+      <c r="BM19" s="10"/>
+      <c r="BN19" s="10"/>
+      <c r="BO19" s="10"/>
+      <c r="BP19" s="10"/>
+      <c r="BQ19" s="10"/>
+      <c r="BR19" s="10"/>
+      <c r="BS19" s="10"/>
+      <c r="BT19" s="10"/>
+      <c r="BU19" s="10"/>
+      <c r="BV19" s="10"/>
+      <c r="BW19" s="10"/>
+      <c r="BX19" s="10"/>
+      <c r="BY19" s="10"/>
+      <c r="BZ19" s="10"/>
+      <c r="CA19" s="10"/>
+      <c r="CB19" s="10"/>
+      <c r="CC19" s="10"/>
+      <c r="CD19" s="10"/>
+    </row>
+    <row r="20" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="str">
         <f>IF(UnitSummary!A23&lt;&gt;"",UnitSummary!A23,"")</f>
         <v/>
@@ -2248,90 +3212,214 @@
         <f>IF(UnitSummary!T23&lt;&gt;"",UnitSummary!T23,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="21" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="str">
+      <c r="U20" s="10"/>
+      <c r="V20" s="10"/>
+      <c r="W20" s="10"/>
+      <c r="X20" s="10"/>
+      <c r="Y20" s="10"/>
+      <c r="Z20" s="10"/>
+      <c r="AA20" s="10"/>
+      <c r="AB20" s="10"/>
+      <c r="AC20" s="10"/>
+      <c r="AD20" s="10"/>
+      <c r="AE20" s="10"/>
+      <c r="AF20" s="10"/>
+      <c r="AG20" s="10"/>
+      <c r="AH20" s="10"/>
+      <c r="AI20" s="10"/>
+      <c r="AJ20" s="10"/>
+      <c r="AK20" s="10"/>
+      <c r="AL20" s="10"/>
+      <c r="AM20" s="10"/>
+      <c r="AN20" s="10"/>
+      <c r="AO20" s="10"/>
+      <c r="AP20" s="10"/>
+      <c r="AQ20" s="10"/>
+      <c r="AR20" s="10"/>
+      <c r="AS20" s="10"/>
+      <c r="AT20" s="10"/>
+      <c r="AU20" s="10"/>
+      <c r="AV20" s="10"/>
+      <c r="AW20" s="10"/>
+      <c r="AX20" s="10"/>
+      <c r="AY20" s="10"/>
+      <c r="AZ20" s="10"/>
+      <c r="BA20" s="10"/>
+      <c r="BB20" s="10"/>
+      <c r="BC20" s="10"/>
+      <c r="BD20" s="10"/>
+      <c r="BE20" s="10"/>
+      <c r="BF20" s="10"/>
+      <c r="BG20" s="10"/>
+      <c r="BH20" s="10"/>
+      <c r="BI20" s="10"/>
+      <c r="BJ20" s="10"/>
+      <c r="BK20" s="10"/>
+      <c r="BL20" s="10"/>
+      <c r="BM20" s="10"/>
+      <c r="BN20" s="10"/>
+      <c r="BO20" s="10"/>
+      <c r="BP20" s="10"/>
+      <c r="BQ20" s="10"/>
+      <c r="BR20" s="10"/>
+      <c r="BS20" s="10"/>
+      <c r="BT20" s="10"/>
+      <c r="BU20" s="10"/>
+      <c r="BV20" s="10"/>
+      <c r="BW20" s="10"/>
+      <c r="BX20" s="10"/>
+      <c r="BY20" s="10"/>
+      <c r="BZ20" s="10"/>
+      <c r="CA20" s="10"/>
+      <c r="CB20" s="10"/>
+      <c r="CC20" s="10"/>
+      <c r="CD20" s="10"/>
+    </row>
+    <row r="21" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="39" t="str">
         <f>IF(UnitSummary!A24&lt;&gt;"",UnitSummary!A24,"")</f>
         <v/>
       </c>
-      <c r="B21" s="2" t="str">
+      <c r="B21" s="39" t="str">
         <f>IF(UnitSummary!B24&lt;&gt;"",UnitSummary!B24,"")</f>
         <v/>
       </c>
-      <c r="C21" s="2" t="str">
+      <c r="C21" s="39" t="str">
         <f>IF(UnitSummary!C24&lt;&gt;"",UnitSummary!C24,"")</f>
         <v/>
       </c>
-      <c r="D21" s="2" t="str">
+      <c r="D21" s="39" t="str">
         <f>IF(UnitSummary!D24&lt;&gt;"",UnitSummary!D24,"")</f>
         <v/>
       </c>
-      <c r="E21" s="2" t="str">
+      <c r="E21" s="39" t="str">
         <f>IF(UnitSummary!E24&lt;&gt;"",UnitSummary!E24,"")</f>
         <v/>
       </c>
-      <c r="F21" s="2" t="str">
+      <c r="F21" s="39" t="str">
         <f>IF(UnitSummary!F24&lt;&gt;"",UnitSummary!F24,"")</f>
         <v/>
       </c>
-      <c r="G21" s="2" t="str">
+      <c r="G21" s="39" t="str">
         <f>IF(UnitSummary!G24&lt;&gt;"",UnitSummary!G24,"")</f>
         <v/>
       </c>
-      <c r="H21" s="2" t="str">
+      <c r="H21" s="39" t="str">
         <f>IF(UnitSummary!H24&lt;&gt;"",UnitSummary!H24,"")</f>
         <v/>
       </c>
-      <c r="I21" s="2" t="str">
+      <c r="I21" s="39" t="str">
         <f>IF(UnitSummary!I24&lt;&gt;"",UnitSummary!I24,"")</f>
         <v/>
       </c>
-      <c r="J21" s="2" t="str">
+      <c r="J21" s="39" t="str">
         <f>IF(UnitSummary!J24&lt;&gt;"",UnitSummary!J24,"")</f>
         <v/>
       </c>
-      <c r="K21" s="2" t="str">
+      <c r="K21" s="39" t="str">
         <f>IF(UnitSummary!K24&lt;&gt;"",UnitSummary!K24,"")</f>
         <v/>
       </c>
-      <c r="L21" s="2" t="str">
+      <c r="L21" s="39" t="str">
         <f>IF(UnitSummary!L24&lt;&gt;"",UnitSummary!L24,"")</f>
         <v/>
       </c>
-      <c r="M21" s="2" t="str">
+      <c r="M21" s="39" t="str">
         <f>IF(UnitSummary!M24&lt;&gt;"",UnitSummary!M24,"")</f>
         <v/>
       </c>
-      <c r="N21" s="2" t="str">
+      <c r="N21" s="39" t="str">
         <f>IF(UnitSummary!N24&lt;&gt;"",UnitSummary!N24,"")</f>
         <v/>
       </c>
-      <c r="O21" s="2" t="str">
+      <c r="O21" s="39" t="str">
         <f>IF(UnitSummary!O24&lt;&gt;"",UnitSummary!O24,"")</f>
         <v/>
       </c>
-      <c r="P21" s="2" t="str">
+      <c r="P21" s="39" t="str">
         <f>IF(UnitSummary!P24&lt;&gt;"",UnitSummary!P24,"")</f>
         <v/>
       </c>
-      <c r="Q21" s="2" t="str">
+      <c r="Q21" s="39" t="str">
         <f>IF(UnitSummary!Q24&lt;&gt;"",UnitSummary!Q24,"")</f>
         <v/>
       </c>
-      <c r="R21" s="2" t="str">
+      <c r="R21" s="39" t="str">
         <f>IF(UnitSummary!R24&lt;&gt;"",UnitSummary!R24,"")</f>
         <v/>
       </c>
-      <c r="S21" s="2" t="str">
+      <c r="S21" s="39" t="str">
         <f>IF(UnitSummary!S24&lt;&gt;"",UnitSummary!S24,"")</f>
         <v/>
       </c>
-      <c r="T21" s="2" t="str">
+      <c r="T21" s="39" t="str">
         <f>IF(UnitSummary!T24&lt;&gt;"",UnitSummary!T24,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="22" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="10"/>
+      <c r="V21" s="10"/>
+      <c r="W21" s="10"/>
+      <c r="X21" s="10"/>
+      <c r="Y21" s="10"/>
+      <c r="Z21" s="10"/>
+      <c r="AA21" s="10"/>
+      <c r="AB21" s="10"/>
+      <c r="AC21" s="10"/>
+      <c r="AD21" s="10"/>
+      <c r="AE21" s="10"/>
+      <c r="AF21" s="10"/>
+      <c r="AG21" s="10"/>
+      <c r="AH21" s="10"/>
+      <c r="AI21" s="10"/>
+      <c r="AJ21" s="10"/>
+      <c r="AK21" s="10"/>
+      <c r="AL21" s="10"/>
+      <c r="AM21" s="10"/>
+      <c r="AN21" s="10"/>
+      <c r="AO21" s="10"/>
+      <c r="AP21" s="10"/>
+      <c r="AQ21" s="10"/>
+      <c r="AR21" s="10"/>
+      <c r="AS21" s="10"/>
+      <c r="AT21" s="10"/>
+      <c r="AU21" s="10"/>
+      <c r="AV21" s="10"/>
+      <c r="AW21" s="10"/>
+      <c r="AX21" s="10"/>
+      <c r="AY21" s="10"/>
+      <c r="AZ21" s="10"/>
+      <c r="BA21" s="10"/>
+      <c r="BB21" s="10"/>
+      <c r="BC21" s="10"/>
+      <c r="BD21" s="10"/>
+      <c r="BE21" s="10"/>
+      <c r="BF21" s="10"/>
+      <c r="BG21" s="10"/>
+      <c r="BH21" s="10"/>
+      <c r="BI21" s="10"/>
+      <c r="BJ21" s="10"/>
+      <c r="BK21" s="10"/>
+      <c r="BL21" s="10"/>
+      <c r="BM21" s="10"/>
+      <c r="BN21" s="10"/>
+      <c r="BO21" s="10"/>
+      <c r="BP21" s="10"/>
+      <c r="BQ21" s="10"/>
+      <c r="BR21" s="10"/>
+      <c r="BS21" s="10"/>
+      <c r="BT21" s="10"/>
+      <c r="BU21" s="10"/>
+      <c r="BV21" s="10"/>
+      <c r="BW21" s="10"/>
+      <c r="BX21" s="10"/>
+      <c r="BY21" s="10"/>
+      <c r="BZ21" s="10"/>
+      <c r="CA21" s="10"/>
+      <c r="CB21" s="10"/>
+      <c r="CC21" s="10"/>
+      <c r="CD21" s="10"/>
+    </row>
+    <row r="22" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="str">
         <f>IF(UnitSummary!A25&lt;&gt;"",UnitSummary!A25,"")</f>
         <v/>
@@ -2412,171 +3500,295 @@
         <f>IF(UnitSummary!T25&lt;&gt;"",UnitSummary!T25,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="23" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2" t="str">
+      <c r="U22" s="10"/>
+      <c r="V22" s="10"/>
+      <c r="W22" s="10"/>
+      <c r="X22" s="10"/>
+      <c r="Y22" s="10"/>
+      <c r="Z22" s="10"/>
+      <c r="AA22" s="10"/>
+      <c r="AB22" s="10"/>
+      <c r="AC22" s="10"/>
+      <c r="AD22" s="10"/>
+      <c r="AE22" s="10"/>
+      <c r="AF22" s="10"/>
+      <c r="AG22" s="10"/>
+      <c r="AH22" s="10"/>
+      <c r="AI22" s="10"/>
+      <c r="AJ22" s="10"/>
+      <c r="AK22" s="10"/>
+      <c r="AL22" s="10"/>
+      <c r="AM22" s="10"/>
+      <c r="AN22" s="10"/>
+      <c r="AO22" s="10"/>
+      <c r="AP22" s="10"/>
+      <c r="AQ22" s="10"/>
+      <c r="AR22" s="10"/>
+      <c r="AS22" s="10"/>
+      <c r="AT22" s="10"/>
+      <c r="AU22" s="10"/>
+      <c r="AV22" s="10"/>
+      <c r="AW22" s="10"/>
+      <c r="AX22" s="10"/>
+      <c r="AY22" s="10"/>
+      <c r="AZ22" s="10"/>
+      <c r="BA22" s="10"/>
+      <c r="BB22" s="10"/>
+      <c r="BC22" s="10"/>
+      <c r="BD22" s="10"/>
+      <c r="BE22" s="10"/>
+      <c r="BF22" s="10"/>
+      <c r="BG22" s="10"/>
+      <c r="BH22" s="10"/>
+      <c r="BI22" s="10"/>
+      <c r="BJ22" s="10"/>
+      <c r="BK22" s="10"/>
+      <c r="BL22" s="10"/>
+      <c r="BM22" s="10"/>
+      <c r="BN22" s="10"/>
+      <c r="BO22" s="10"/>
+      <c r="BP22" s="10"/>
+      <c r="BQ22" s="10"/>
+      <c r="BR22" s="10"/>
+      <c r="BS22" s="10"/>
+      <c r="BT22" s="10"/>
+      <c r="BU22" s="10"/>
+      <c r="BV22" s="10"/>
+      <c r="BW22" s="10"/>
+      <c r="BX22" s="10"/>
+      <c r="BY22" s="10"/>
+      <c r="BZ22" s="10"/>
+      <c r="CA22" s="10"/>
+      <c r="CB22" s="10"/>
+      <c r="CC22" s="10"/>
+      <c r="CD22" s="10"/>
+    </row>
+    <row r="23" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="39" t="str">
         <f>IF(UnitSummary!A26&lt;&gt;"",UnitSummary!A26,"")</f>
         <v/>
       </c>
-      <c r="B23" s="2" t="str">
+      <c r="B23" s="39" t="str">
         <f>IF(UnitSummary!B26&lt;&gt;"",UnitSummary!B26,"")</f>
         <v/>
       </c>
-      <c r="C23" s="2" t="str">
+      <c r="C23" s="39" t="str">
         <f>IF(UnitSummary!C26&lt;&gt;"",UnitSummary!C26,"")</f>
         <v/>
       </c>
-      <c r="D23" s="2" t="str">
+      <c r="D23" s="39" t="str">
         <f>IF(UnitSummary!D26&lt;&gt;"",UnitSummary!D26,"")</f>
         <v/>
       </c>
-      <c r="E23" s="2" t="str">
+      <c r="E23" s="39" t="str">
         <f>IF(UnitSummary!E26&lt;&gt;"",UnitSummary!E26,"")</f>
         <v/>
       </c>
-      <c r="F23" s="2" t="str">
+      <c r="F23" s="39" t="str">
         <f>IF(UnitSummary!F26&lt;&gt;"",UnitSummary!F26,"")</f>
         <v/>
       </c>
-      <c r="G23" s="2" t="str">
+      <c r="G23" s="39" t="str">
         <f>IF(UnitSummary!G26&lt;&gt;"",UnitSummary!G26,"")</f>
         <v/>
       </c>
-      <c r="H23" s="2" t="str">
+      <c r="H23" s="39" t="str">
         <f>IF(UnitSummary!H26&lt;&gt;"",UnitSummary!H26,"")</f>
         <v/>
       </c>
-      <c r="I23" s="2" t="str">
+      <c r="I23" s="39" t="str">
         <f>IF(UnitSummary!I26&lt;&gt;"",UnitSummary!I26,"")</f>
         <v/>
       </c>
-      <c r="J23" s="2" t="str">
+      <c r="J23" s="39" t="str">
         <f>IF(UnitSummary!J26&lt;&gt;"",UnitSummary!J26,"")</f>
         <v/>
       </c>
-      <c r="K23" s="2" t="str">
+      <c r="K23" s="39" t="str">
         <f>IF(UnitSummary!K26&lt;&gt;"",UnitSummary!K26,"")</f>
         <v/>
       </c>
-      <c r="L23" s="2" t="str">
+      <c r="L23" s="39" t="str">
         <f>IF(UnitSummary!L26&lt;&gt;"",UnitSummary!L26,"")</f>
         <v/>
       </c>
-      <c r="M23" s="2" t="str">
+      <c r="M23" s="39" t="str">
         <f>IF(UnitSummary!M26&lt;&gt;"",UnitSummary!M26,"")</f>
         <v/>
       </c>
-      <c r="N23" s="2" t="str">
+      <c r="N23" s="39" t="str">
         <f>IF(UnitSummary!N26&lt;&gt;"",UnitSummary!N26,"")</f>
         <v/>
       </c>
-      <c r="O23" s="2" t="str">
+      <c r="O23" s="39" t="str">
         <f>IF(UnitSummary!O26&lt;&gt;"",UnitSummary!O26,"")</f>
         <v/>
       </c>
-      <c r="P23" s="2" t="str">
+      <c r="P23" s="39" t="str">
         <f>IF(UnitSummary!P26&lt;&gt;"",UnitSummary!P26,"")</f>
         <v/>
       </c>
-      <c r="Q23" s="2" t="str">
+      <c r="Q23" s="39" t="str">
         <f>IF(UnitSummary!Q26&lt;&gt;"",UnitSummary!Q26,"")</f>
         <v/>
       </c>
-      <c r="R23" s="2" t="str">
+      <c r="R23" s="39" t="str">
         <f>IF(UnitSummary!R26&lt;&gt;"",UnitSummary!R26,"")</f>
         <v/>
       </c>
-      <c r="S23" s="2" t="str">
+      <c r="S23" s="39" t="str">
         <f>IF(UnitSummary!S26&lt;&gt;"",UnitSummary!S26,"")</f>
         <v/>
       </c>
-      <c r="T23" s="2" t="str">
+      <c r="T23" s="39" t="str">
         <f>IF(UnitSummary!T26&lt;&gt;"",UnitSummary!T26,"")</f>
         <v/>
       </c>
-    </row>
-    <row r="24" spans="1:22" s="41" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="40" t="s">
+      <c r="U23" s="10"/>
+      <c r="V23" s="10"/>
+      <c r="W23" s="10"/>
+      <c r="X23" s="10"/>
+      <c r="Y23" s="10"/>
+      <c r="Z23" s="10"/>
+      <c r="AA23" s="10"/>
+      <c r="AB23" s="10"/>
+      <c r="AC23" s="10"/>
+      <c r="AD23" s="10"/>
+      <c r="AE23" s="10"/>
+      <c r="AF23" s="10"/>
+      <c r="AG23" s="10"/>
+      <c r="AH23" s="10"/>
+      <c r="AI23" s="10"/>
+      <c r="AJ23" s="10"/>
+      <c r="AK23" s="10"/>
+      <c r="AL23" s="10"/>
+      <c r="AM23" s="10"/>
+      <c r="AN23" s="10"/>
+      <c r="AO23" s="10"/>
+      <c r="AP23" s="10"/>
+      <c r="AQ23" s="10"/>
+      <c r="AR23" s="10"/>
+      <c r="AS23" s="10"/>
+      <c r="AT23" s="10"/>
+      <c r="AU23" s="10"/>
+      <c r="AV23" s="10"/>
+      <c r="AW23" s="10"/>
+      <c r="AX23" s="10"/>
+      <c r="AY23" s="10"/>
+      <c r="AZ23" s="10"/>
+      <c r="BA23" s="10"/>
+      <c r="BB23" s="10"/>
+      <c r="BC23" s="10"/>
+      <c r="BD23" s="10"/>
+      <c r="BE23" s="10"/>
+      <c r="BF23" s="10"/>
+      <c r="BG23" s="10"/>
+      <c r="BH23" s="10"/>
+      <c r="BI23" s="10"/>
+      <c r="BJ23" s="10"/>
+      <c r="BK23" s="10"/>
+      <c r="BL23" s="10"/>
+      <c r="BM23" s="10"/>
+      <c r="BN23" s="10"/>
+      <c r="BO23" s="10"/>
+      <c r="BP23" s="10"/>
+      <c r="BQ23" s="10"/>
+      <c r="BR23" s="10"/>
+      <c r="BS23" s="10"/>
+      <c r="BT23" s="10"/>
+      <c r="BU23" s="10"/>
+      <c r="BV23" s="10"/>
+      <c r="BW23" s="10"/>
+      <c r="BX23" s="10"/>
+      <c r="BY23" s="10"/>
+      <c r="BZ23" s="10"/>
+      <c r="CA23" s="10"/>
+      <c r="CB23" s="10"/>
+      <c r="CC23" s="10"/>
+      <c r="CD23" s="10"/>
+    </row>
+    <row r="24" spans="1:82" s="26" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="40">
+      <c r="B24" s="25">
         <f>IF(SUM(B4:B23)&lt;&gt;0,SUM(B4:B23),"")</f>
         <v>10</v>
       </c>
-      <c r="C24" s="40">
+      <c r="C24" s="25">
         <f t="shared" ref="C24:Q24" si="0">IF(SUM(C4:C23)&lt;&gt;0,SUM(C4:C23),"")</f>
         <v>4</v>
       </c>
-      <c r="D24" s="40">
+      <c r="D24" s="25">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="E24" s="40">
+      <c r="E24" s="25">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="F24" s="40" t="str">
+      <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="G24" s="40" t="str">
+      <c r="G24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="H24" s="40" t="str">
+      <c r="H24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="I24" s="40" t="str">
+      <c r="I24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="J24" s="40" t="str">
+      <c r="J24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="K24" s="40" t="str">
+      <c r="K24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="L24" s="40" t="str">
+      <c r="L24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="M24" s="40" t="str">
+      <c r="M24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="N24" s="40" t="str">
+      <c r="N24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="O24" s="40" t="str">
+      <c r="O24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="P24" s="40" t="str">
+      <c r="P24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="Q24" s="40" t="str">
+      <c r="Q24" s="25" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
-      <c r="R24" s="40" t="str">
+      <c r="R24" s="25" t="str">
         <f t="shared" ref="R24" si="1">IF(SUM(R4:R23)&lt;&gt;0,SUM(R4:R23),"")</f>
         <v/>
       </c>
-      <c r="S24" s="40" t="str">
+      <c r="S24" s="25" t="str">
         <f t="shared" ref="S24" si="2">IF(SUM(S4:S23)&lt;&gt;0,SUM(S4:S23),"")</f>
         <v/>
       </c>
-      <c r="T24" s="40" t="str">
+      <c r="T24" s="25" t="str">
         <f t="shared" ref="T24" si="3">IF(SUM(T4:T23)&lt;&gt;0,SUM(T4:T23),"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
         <v>3</v>
       </c>
@@ -2646,20 +3858,20 @@
       </c>
       <c r="U25" s="6"/>
     </row>
-    <row r="26" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" s="7">
-        <f>B24/L31</f>
+        <f>B24/B29</f>
         <v>0.55555555555555558</v>
       </c>
       <c r="C26" s="7">
-        <f>C24/L31</f>
+        <f>C24/B29</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="D26" s="7">
-        <f>D24/L31</f>
+        <f>D24/B29</f>
         <v>0.22222222222222221</v>
       </c>
       <c r="E26" s="7"/>
@@ -2680,9 +3892,9 @@
       <c r="T26" s="7"/>
       <c r="U26" s="7"/>
     </row>
-    <row r="27" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B27" s="11">
         <f>B25*B24</f>
@@ -2714,148 +3926,268 @@
       <c r="T27" s="11"/>
       <c r="U27" s="11"/>
     </row>
-    <row r="28" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="5"/>
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="13"/>
-      <c r="F28" s="13"/>
-      <c r="G28" s="7"/>
-      <c r="H28" s="7"/>
-      <c r="I28" s="7"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="7"/>
-      <c r="L28" s="7"/>
-      <c r="M28" s="7"/>
-      <c r="N28" s="7"/>
-      <c r="O28" s="7"/>
-      <c r="P28" s="7"/>
-      <c r="Q28" s="7"/>
-      <c r="R28" s="7"/>
-      <c r="S28" s="7"/>
-      <c r="T28" s="7"/>
-      <c r="U28" s="7"/>
-    </row>
-    <row r="29" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="19"/>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="14"/>
-      <c r="I29" s="19"/>
-      <c r="M29" s="6"/>
-      <c r="N29" s="6"/>
-      <c r="O29" s="6"/>
-      <c r="P29" s="6"/>
-      <c r="Q29" s="6"/>
-      <c r="R29" s="6"/>
-      <c r="S29" s="14"/>
-      <c r="U29" s="17"/>
-    </row>
-    <row r="30" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="35" t="s">
+      <c r="B28" s="11"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="11"/>
+      <c r="E28" s="11"/>
+      <c r="F28" s="11"/>
+      <c r="G28" s="11"/>
+      <c r="H28" s="11"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="11"/>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11"/>
+      <c r="M28" s="11"/>
+      <c r="N28" s="11"/>
+      <c r="O28" s="11"/>
+      <c r="P28" s="11"/>
+      <c r="Q28" s="11"/>
+      <c r="R28" s="11"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
+      <c r="U28" s="11"/>
+    </row>
+    <row r="29" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B29" s="29">
+        <f>E24</f>
+        <v>18</v>
+      </c>
+      <c r="C29" s="7"/>
+      <c r="D29" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="B30" s="20">
-        <f>SUM(B24:F24)</f>
-        <v>36</v>
-      </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="22">
-        <f>SUM(G24:H24)</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="21"/>
-      <c r="F30" s="25">
-        <f>SUM(I24:I24)</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="23"/>
-      <c r="H30" s="30">
-        <f>SUM(J24:M24)</f>
-        <v>0</v>
-      </c>
-      <c r="I30" s="24"/>
-      <c r="J30" s="26">
-        <f>SUM(N24:Q24)</f>
-        <v>0</v>
-      </c>
-      <c r="L30" s="38" t="s">
+      <c r="E29" s="13"/>
+      <c r="F29" s="9">
+        <f>B30/B29</f>
+        <v>266.66666666666669</v>
+      </c>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+    </row>
+    <row r="30" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="5" t="s">
         <v>17</v>
       </c>
+      <c r="B30" s="30">
+        <f>SUM(27:27)</f>
+        <v>4800</v>
+      </c>
+      <c r="C30" s="19"/>
+      <c r="D30" s="19"/>
+      <c r="E30" s="19"/>
+      <c r="F30" s="19"/>
+      <c r="G30" s="19"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="19"/>
       <c r="M30" s="6"/>
-      <c r="N30" s="6" t="s">
-        <v>10</v>
-      </c>
+      <c r="N30" s="6"/>
       <c r="O30" s="6"/>
       <c r="P30" s="6"/>
       <c r="Q30" s="6"/>
       <c r="R30" s="6"/>
-      <c r="S30" s="9"/>
-      <c r="U30" s="18"/>
-      <c r="V30" s="8"/>
-    </row>
-    <row r="31" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="3"/>
-      <c r="B31" s="27" t="e">
-        <f>B30/R24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="29" t="e">
-        <f>D30/R24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="E31" s="28"/>
-      <c r="F31" s="31" t="e">
-        <f>F30/R24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="G31" s="23"/>
-      <c r="H31" s="31" t="e">
-        <f>H30/R24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="I31" s="24"/>
-      <c r="J31" s="32" t="e">
-        <f>SUM(N24:Q24)/R24</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="L31" s="39">
-        <f>E24</f>
-        <v>18</v>
-      </c>
-      <c r="N31" s="6" t="e">
-        <f>R27/R24</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="32" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="3"/>
-      <c r="B32" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" s="16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H32" s="16" t="s">
-        <v>12</v>
-      </c>
-      <c r="I32"/>
-      <c r="J32" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="N32" s="37" t="e">
-        <f>SUM(B31:J31)</f>
-        <v>#VALUE!</v>
-      </c>
+      <c r="S30" s="14"/>
+      <c r="U30" s="17"/>
+    </row>
+    <row r="31" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="O31" s="6"/>
+      <c r="P31" s="6"/>
+      <c r="Q31" s="6"/>
+      <c r="R31" s="6"/>
+      <c r="S31" s="9"/>
+      <c r="U31" s="18"/>
+      <c r="V31" s="8"/>
+    </row>
+    <row r="32" spans="1:82" s="41" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="53" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="44" t="str">
+        <f>IF(UnitMix!A1&lt;&gt;"",UnitMix!A1,"")</f>
+        <v>Open 1 Bedroom</v>
+      </c>
+      <c r="C32" s="47" t="str">
+        <f>IF(UnitMix!B1&lt;&gt;"",UnitMix!B1,"")</f>
+        <v>1 Bedroom + Den</v>
+      </c>
+      <c r="D32" s="50" t="str">
+        <f>IF(UnitMix!C1&lt;&gt;"",UnitMix!C1,"")</f>
+        <v>2 Bedroom</v>
+      </c>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="42" t="str">
+        <f>IF(UnitMix!J1&lt;&gt;"",UnitMix!J1,"")</f>
+        <v/>
+      </c>
+      <c r="L32" s="42" t="str">
+        <f>IF(UnitMix!K1&lt;&gt;"",UnitMix!K1,"")</f>
+        <v/>
+      </c>
+      <c r="M32" s="42" t="str">
+        <f>IF(UnitMix!L1&lt;&gt;"",UnitMix!L1,"")</f>
+        <v/>
+      </c>
+      <c r="N32" s="42" t="str">
+        <f>IF(UnitMix!M1&lt;&gt;"",UnitMix!M1,"")</f>
+        <v/>
+      </c>
+      <c r="O32" s="42" t="str">
+        <f>IF(UnitMix!N1&lt;&gt;"",UnitMix!N1,"")</f>
+        <v/>
+      </c>
+      <c r="P32" s="42" t="str">
+        <f>IF(UnitMix!O1&lt;&gt;"",UnitMix!O1,"")</f>
+        <v/>
+      </c>
+      <c r="Q32" s="42" t="str">
+        <f>IF(UnitMix!P1&lt;&gt;"",UnitMix!P1,"")</f>
+        <v/>
+      </c>
+      <c r="R32" s="42" t="str">
+        <f>IF(UnitMix!Q1&lt;&gt;"",UnitMix!Q1,"")</f>
+        <v/>
+      </c>
+      <c r="S32" s="42" t="str">
+        <f>IF(UnitMix!R1&lt;&gt;"",UnitMix!R1,"")</f>
+        <v/>
+      </c>
+      <c r="T32" s="42" t="str">
+        <f>IF(UnitMix!S1&lt;&gt;"",UnitMix!S1,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="45">
+        <f>IF(UnitMix!A2&lt;&gt;"",UnitMix!A2,"")</f>
+        <v>10</v>
+      </c>
+      <c r="C33" s="48">
+        <f>IF(UnitMix!B2&lt;&gt;"",UnitMix!B2,"")</f>
+        <v>4</v>
+      </c>
+      <c r="D33" s="51">
+        <f>IF(UnitMix!C2&lt;&gt;"",UnitMix!C2,"")</f>
+        <v>4</v>
+      </c>
+      <c r="E33" s="33" t="str">
+        <f>IF(UnitMix!D2&lt;&gt;"",UnitMix!D2,"")</f>
+        <v/>
+      </c>
+      <c r="F33" s="33" t="str">
+        <f>IF(UnitMix!E2&lt;&gt;"",UnitMix!E2,"")</f>
+        <v/>
+      </c>
+      <c r="G33" s="33" t="str">
+        <f>IF(UnitMix!F2&lt;&gt;"",UnitMix!F2,"")</f>
+        <v/>
+      </c>
+      <c r="H33" s="33" t="str">
+        <f>IF(UnitMix!G2&lt;&gt;"",UnitMix!G2,"")</f>
+        <v/>
+      </c>
+      <c r="I33" s="33" t="str">
+        <f>IF(UnitMix!H2&lt;&gt;"",UnitMix!H2,"")</f>
+        <v/>
+      </c>
+      <c r="J33" s="33" t="str">
+        <f>IF(UnitMix!I2&lt;&gt;"",UnitMix!I2,"")</f>
+        <v/>
+      </c>
+      <c r="K33" s="33" t="str">
+        <f>IF(UnitMix!J2&lt;&gt;"",UnitMix!J2,"")</f>
+        <v/>
+      </c>
+      <c r="L33" s="33" t="str">
+        <f>IF(UnitMix!K2&lt;&gt;"",UnitMix!K2,"")</f>
+        <v/>
+      </c>
+      <c r="M33" s="33" t="str">
+        <f>IF(UnitMix!L2&lt;&gt;"",UnitMix!L2,"")</f>
+        <v/>
+      </c>
+      <c r="N33" s="33" t="str">
+        <f>IF(UnitMix!M2&lt;&gt;"",UnitMix!M2,"")</f>
+        <v/>
+      </c>
+      <c r="O33" s="33" t="str">
+        <f>IF(UnitMix!N2&lt;&gt;"",UnitMix!N2,"")</f>
+        <v/>
+      </c>
+      <c r="P33" s="33" t="str">
+        <f>IF(UnitMix!O2&lt;&gt;"",UnitMix!O2,"")</f>
+        <v/>
+      </c>
+      <c r="Q33" s="33" t="str">
+        <f>IF(UnitMix!P2&lt;&gt;"",UnitMix!P2,"")</f>
+        <v/>
+      </c>
+      <c r="R33" s="33" t="str">
+        <f>IF(UnitMix!Q2&lt;&gt;"",UnitMix!Q2,"")</f>
+        <v/>
+      </c>
+      <c r="S33" s="33" t="str">
+        <f>IF(UnitMix!R2&lt;&gt;"",UnitMix!R2,"")</f>
+        <v/>
+      </c>
+      <c r="T33" s="33" t="str">
+        <f>IF(UnitMix!S2&lt;&gt;"",UnitMix!S2,"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A34" s="3"/>
+      <c r="B34" s="46">
+        <f>B33/B29</f>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="C34" s="49">
+        <f>C33/B29</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D34" s="52">
+        <f>D33/B29</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E34" s="35"/>
+      <c r="F34" s="37"/>
+      <c r="G34" s="34"/>
+      <c r="H34" s="37"/>
+      <c r="I34" s="36"/>
+      <c r="J34" s="38"/>
+      <c r="L34" s="24"/>
+      <c r="N34" s="6"/>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A35" s="3"/>
+      <c r="B35" s="20"/>
+      <c r="D35" s="21"/>
+      <c r="F35" s="16"/>
+      <c r="H35" s="16"/>
+      <c r="I35"/>
+      <c r="J35" s="12"/>
+      <c r="N35" s="23"/>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -2874,25 +4206,25 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B2">
         <v>200</v>
@@ -2906,7 +4238,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -2920,7 +4252,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -2934,7 +4266,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2965,7 +4297,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>5</v>
@@ -2982,7 +4314,7 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>5</v>
@@ -3004,14 +4336,37 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
cleanup and upgrade to Dynamo 9.1
</commit_message>
<xml_diff>
--- a/sandbox/Yield Matrix - Copy.xlsx
+++ b/sandbox/Yield Matrix - Copy.xlsx
@@ -24,15 +24,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>TOTAL</t>
   </si>
   <si>
     <t>UNIT SUMMARY</t>
-  </si>
-  <si>
-    <t>FLOOR</t>
   </si>
   <si>
     <t>Unit Area (+/-)</t>
@@ -47,34 +44,7 @@
     <t>Average Unit Area</t>
   </si>
   <si>
-    <t>Open 1 Bedroom</t>
-  </si>
-  <si>
-    <t>2 Bedroom</t>
-  </si>
-  <si>
-    <t>Level 1</t>
-  </si>
-  <si>
-    <t>Level 2</t>
-  </si>
-  <si>
     <t>Total Units</t>
-  </si>
-  <si>
-    <t>1 Bedroom + Den</t>
-  </si>
-  <si>
-    <t>Area</t>
-  </si>
-  <si>
-    <t>Bedrooms</t>
-  </si>
-  <si>
-    <t>Baths</t>
-  </si>
-  <si>
-    <t>Den</t>
   </si>
   <si>
     <t>Total Rentable Area</t>
@@ -704,7 +674,7 @@
   <dimension ref="A1:CD35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K31" sqref="J31:K31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,15 +702,15 @@
       </c>
       <c r="B2" s="27" t="str">
         <f>IF(UnitSummary!B1&lt;&gt;"",UnitSummary!B1,"")</f>
-        <v>Open 1 Bedroom</v>
+        <v/>
       </c>
       <c r="C2" s="27" t="str">
         <f>IF(UnitSummary!C1&lt;&gt;"",UnitSummary!C1,"")</f>
-        <v>1 Bedroom + Den</v>
+        <v/>
       </c>
       <c r="D2" s="27" t="str">
         <f>IF(UnitSummary!D1&lt;&gt;"",UnitSummary!D1,"")</f>
-        <v>2 Bedroom</v>
+        <v/>
       </c>
       <c r="E2" s="27" t="str">
         <f>IF(UnitSummary!E1&lt;&gt;"",UnitSummary!E1,"")</f>
@@ -810,23 +780,23 @@
     <row r="3" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="str">
         <f>IF(UnitSummary!A6&lt;&gt;"",UnitSummary!A6,"")</f>
-        <v>FLOOR</v>
-      </c>
-      <c r="B3" s="22">
+        <v/>
+      </c>
+      <c r="B3" s="22" t="str">
         <f>IF(UnitSummary!B6&lt;&gt;"",UnitSummary!B6,"")</f>
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C3" s="22">
+        <v/>
+      </c>
+      <c r="C3" s="22" t="str">
         <f>IF(UnitSummary!C6&lt;&gt;"",UnitSummary!C6,"")</f>
-        <v>1.2</v>
-      </c>
-      <c r="D3" s="22">
+        <v/>
+      </c>
+      <c r="D3" s="22" t="str">
         <f>IF(UnitSummary!D6&lt;&gt;"",UnitSummary!D6,"")</f>
-        <v>2.1</v>
+        <v/>
       </c>
       <c r="E3" s="22" t="str">
         <f>IF(UnitSummary!E6&lt;&gt;"",UnitSummary!E6,"")</f>
-        <v>TOTAL</v>
+        <v/>
       </c>
       <c r="F3" s="22" t="str">
         <f>IF(UnitSummary!F6&lt;&gt;"",UnitSummary!F6,"")</f>
@@ -892,23 +862,23 @@
     <row r="4" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="str">
         <f>IF(UnitSummary!A7&lt;&gt;"",UnitSummary!A7,"")</f>
-        <v>Level 1</v>
-      </c>
-      <c r="B4" s="2">
+        <v/>
+      </c>
+      <c r="B4" s="2" t="str">
         <f>IF(UnitSummary!B7&lt;&gt;"",UnitSummary!B7,"")</f>
-        <v>5</v>
-      </c>
-      <c r="C4" s="2">
+        <v/>
+      </c>
+      <c r="C4" s="2" t="str">
         <f>IF(UnitSummary!C7&lt;&gt;"",UnitSummary!C7,"")</f>
-        <v>2</v>
-      </c>
-      <c r="D4" s="2">
+        <v/>
+      </c>
+      <c r="D4" s="2" t="str">
         <f>IF(UnitSummary!D7&lt;&gt;"",UnitSummary!D7,"")</f>
-        <v>2</v>
-      </c>
-      <c r="E4" s="2">
+        <v/>
+      </c>
+      <c r="E4" s="2" t="str">
         <f>IF(UnitSummary!E7&lt;&gt;"",UnitSummary!E7,"")</f>
-        <v>9</v>
+        <v/>
       </c>
       <c r="F4" s="2" t="str">
         <f>IF(UnitSummary!F7&lt;&gt;"",UnitSummary!F7,"")</f>
@@ -974,23 +944,23 @@
     <row r="5" spans="1:82" s="40" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="str">
         <f>IF(UnitSummary!A8&lt;&gt;"",UnitSummary!A8,"")</f>
-        <v>Level 2</v>
-      </c>
-      <c r="B5" s="39">
+        <v/>
+      </c>
+      <c r="B5" s="39" t="str">
         <f>IF(UnitSummary!B8&lt;&gt;"",UnitSummary!B8,"")</f>
-        <v>5</v>
-      </c>
-      <c r="C5" s="39">
+        <v/>
+      </c>
+      <c r="C5" s="39" t="str">
         <f>IF(UnitSummary!C8&lt;&gt;"",UnitSummary!C8,"")</f>
-        <v>2</v>
-      </c>
-      <c r="D5" s="39">
+        <v/>
+      </c>
+      <c r="D5" s="39" t="str">
         <f>IF(UnitSummary!D8&lt;&gt;"",UnitSummary!D8,"")</f>
-        <v>2</v>
-      </c>
-      <c r="E5" s="39">
+        <v/>
+      </c>
+      <c r="E5" s="39" t="str">
         <f>IF(UnitSummary!E8&lt;&gt;"",UnitSummary!E8,"")</f>
-        <v>9</v>
+        <v/>
       </c>
       <c r="F5" s="39" t="str">
         <f>IF(UnitSummary!F8&lt;&gt;"",UnitSummary!F8,"")</f>
@@ -3711,21 +3681,21 @@
       <c r="A24" s="31" t="s">
         <v>0</v>
       </c>
-      <c r="B24" s="25">
-        <f>IF(SUM(B4:B23)&lt;&gt;0,SUM(B4:B23),"")</f>
-        <v>10</v>
-      </c>
-      <c r="C24" s="25">
-        <f t="shared" ref="C24:Q24" si="0">IF(SUM(C4:C23)&lt;&gt;0,SUM(C4:C23),"")</f>
-        <v>4</v>
-      </c>
-      <c r="D24" s="25">
+      <c r="B24" s="25" t="str">
+        <f t="shared" ref="B24:T24" si="0">IF(SUM(B4:B23)&lt;&gt;0,SUM(B4:B23),"")</f>
+        <v/>
+      </c>
+      <c r="C24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="E24" s="25">
+        <v/>
+      </c>
+      <c r="D24" s="25" t="str">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v/>
+      </c>
+      <c r="E24" s="25" t="str">
+        <f t="shared" si="0"/>
+        <v/>
       </c>
       <c r="F24" s="25" t="str">
         <f t="shared" si="0"/>
@@ -3776,33 +3746,33 @@
         <v/>
       </c>
       <c r="R24" s="25" t="str">
-        <f t="shared" ref="R24" si="1">IF(SUM(R4:R23)&lt;&gt;0,SUM(R4:R23),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="S24" s="25" t="str">
-        <f t="shared" ref="S24" si="2">IF(SUM(S4:S23)&lt;&gt;0,SUM(S4:S23),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="T24" s="25" t="str">
-        <f t="shared" ref="T24" si="3">IF(SUM(T4:T23)&lt;&gt;0,SUM(T4:T23),"")</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
     </row>
     <row r="25" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B25" s="15">
+        <v>2</v>
+      </c>
+      <c r="B25" s="15" t="str">
         <f>IF(UnitSummary!B2&lt;&gt;"",UnitSummary!B2,"")</f>
-        <v>200</v>
-      </c>
-      <c r="C25" s="15">
+        <v/>
+      </c>
+      <c r="C25" s="15" t="str">
         <f>IF(UnitSummary!C2&lt;&gt;"",UnitSummary!C2,"")</f>
-        <v>300</v>
-      </c>
-      <c r="D25" s="15">
+        <v/>
+      </c>
+      <c r="D25" s="15" t="str">
         <f>IF(UnitSummary!D2&lt;&gt;"",UnitSummary!D2,"")</f>
-        <v>400</v>
+        <v/>
       </c>
       <c r="E25" s="15" t="str">
         <f>IF(UnitSummary!E2&lt;&gt;"",UnitSummary!E2,"")</f>
@@ -3860,19 +3830,19 @@
     </row>
     <row r="26" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B26" s="7">
+        <v>3</v>
+      </c>
+      <c r="B26" s="7" t="e">
         <f>B24/B29</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C26" s="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C26" s="7" t="e">
         <f>C24/B29</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D26" s="7">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D26" s="7" t="e">
         <f>D24/B29</f>
-        <v>0.22222222222222221</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
@@ -3894,19 +3864,19 @@
     </row>
     <row r="27" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B27" s="11">
+        <v>8</v>
+      </c>
+      <c r="B27" s="11" t="e">
         <f>B25*B24</f>
-        <v>2000</v>
-      </c>
-      <c r="C27" s="11">
-        <f>C25*C24</f>
-        <v>1200</v>
-      </c>
-      <c r="D27" s="11">
-        <f>D25*D24</f>
-        <v>1600</v>
+        <v>#VALUE!</v>
+      </c>
+      <c r="C27" s="11" t="e">
+        <f t="shared" ref="C27:D27" si="1">C25*C24</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D27" s="11" t="e">
+        <f t="shared" si="1"/>
+        <v>#VALUE!</v>
       </c>
       <c r="E27" s="11"/>
       <c r="F27" s="11"/>
@@ -3951,20 +3921,20 @@
     </row>
     <row r="29" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="29">
+        <v>6</v>
+      </c>
+      <c r="B29" s="29" t="str">
         <f>E24</f>
-        <v>18</v>
+        <v/>
       </c>
       <c r="C29" s="7"/>
       <c r="D29" s="32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E29" s="13"/>
-      <c r="F29" s="9">
+      <c r="F29" s="9" t="e">
         <f>B30/B29</f>
-        <v>266.66666666666669</v>
+        <v>#VALUE!</v>
       </c>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
@@ -3984,11 +3954,11 @@
     </row>
     <row r="30" spans="1:82" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B30" s="30">
+        <v>7</v>
+      </c>
+      <c r="B30" s="30" t="e">
         <f>SUM(27:27)</f>
-        <v>4800</v>
+        <v>#VALUE!</v>
       </c>
       <c r="C30" s="19"/>
       <c r="D30" s="19"/>
@@ -4017,19 +3987,19 @@
     </row>
     <row r="32" spans="1:82" s="41" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="53" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B32" s="44" t="str">
         <f>IF(UnitMix!A1&lt;&gt;"",UnitMix!A1,"")</f>
-        <v>Open 1 Bedroom</v>
+        <v/>
       </c>
       <c r="C32" s="47" t="str">
         <f>IF(UnitMix!B1&lt;&gt;"",UnitMix!B1,"")</f>
-        <v>1 Bedroom + Den</v>
+        <v/>
       </c>
       <c r="D32" s="50" t="str">
         <f>IF(UnitMix!C1&lt;&gt;"",UnitMix!C1,"")</f>
-        <v>2 Bedroom</v>
+        <v/>
       </c>
       <c r="E32" s="43"/>
       <c r="F32" s="43"/>
@@ -4079,17 +4049,17 @@
       </c>
     </row>
     <row r="33" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="45">
+      <c r="B33" s="45" t="str">
         <f>IF(UnitMix!A2&lt;&gt;"",UnitMix!A2,"")</f>
-        <v>10</v>
-      </c>
-      <c r="C33" s="48">
+        <v/>
+      </c>
+      <c r="C33" s="48" t="str">
         <f>IF(UnitMix!B2&lt;&gt;"",UnitMix!B2,"")</f>
-        <v>4</v>
-      </c>
-      <c r="D33" s="51">
+        <v/>
+      </c>
+      <c r="D33" s="51" t="str">
         <f>IF(UnitMix!C2&lt;&gt;"",UnitMix!C2,"")</f>
-        <v>4</v>
+        <v/>
       </c>
       <c r="E33" s="33" t="str">
         <f>IF(UnitMix!D2&lt;&gt;"",UnitMix!D2,"")</f>
@@ -4158,17 +4128,17 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A34" s="3"/>
-      <c r="B34" s="46">
+      <c r="B34" s="46" t="e">
         <f>B33/B29</f>
-        <v>0.55555555555555558</v>
-      </c>
-      <c r="C34" s="49">
+        <v>#VALUE!</v>
+      </c>
+      <c r="C34" s="49" t="e">
         <f>C33/B29</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D34" s="52">
+        <v>#VALUE!</v>
+      </c>
+      <c r="D34" s="52" t="e">
         <f>D33/B29</f>
-        <v>0.22222222222222221</v>
+        <v>#VALUE!</v>
       </c>
       <c r="E34" s="35"/>
       <c r="F34" s="37"/>
@@ -4203,170 +4173,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="G11" sqref="A1:G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2">
-        <v>200</v>
-      </c>
-      <c r="C2">
-        <v>300</v>
-      </c>
-      <c r="D2">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C6">
-        <v>1.2</v>
-      </c>
-      <c r="D6">
-        <v>2.1</v>
-      </c>
-      <c r="E6" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>5</v>
-      </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7">
-        <v>2</v>
-      </c>
-      <c r="E7">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>2</v>
-      </c>
-      <c r="E8">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>4</v>
-      </c>
-      <c r="C2">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>